<commit_message>
added desc56 octave tables
</commit_message>
<xml_diff>
--- a/Paper/ir_expansion_diagrams.xlsx
+++ b/Paper/ir_expansion_diagrams.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilanashapiro/Documents/CS132/MusAssist/Paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B05D6F28-F2F2-0E4D-A697-1A591B834CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D6AD74-7FA3-D944-8A93-5B1EC2B38314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{9CC0B3E8-72D6-5245-A968-31A972243904}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="81">
   <si>
     <t>C</t>
   </si>
@@ -195,6 +195,103 @@
   <si>
     <t>desc56</t>
   </si>
+  <si>
+    <t>pred</t>
+  </si>
+  <si>
+    <t>pred2</t>
+  </si>
+  <si>
+    <t>succ</t>
+  </si>
+  <si>
+    <t>2,4,6
+7,9,11</t>
+  </si>
+  <si>
+    <t>8,10,12
+13</t>
+  </si>
+  <si>
+    <t>2,4,6,8
+7,9,11,13</t>
+  </si>
+  <si>
+    <t>10,12</t>
+  </si>
+  <si>
+    <t>1,3</t>
+  </si>
+  <si>
+    <t>4,6,8
+9,11,13</t>
+  </si>
+  <si>
+    <t>4,6,8,10
+9,11,13</t>
+  </si>
+  <si>
+    <t>6,8,10
+11,13</t>
+  </si>
+  <si>
+    <t>6,8,10,12
+11,13</t>
+  </si>
+  <si>
+    <t>Desc 56</t>
+  </si>
+  <si>
+    <t>C,D</t>
+  </si>
+  <si>
+    <t>C,D,E,F</t>
+  </si>
+  <si>
+    <t>C,D,E,F,G,A</t>
+  </si>
+  <si>
+    <t>D,E,F,G,A,B</t>
+  </si>
+  <si>
+    <t>F,G,A,B</t>
+  </si>
+  <si>
+    <t>A,B</t>
+  </si>
+  <si>
+    <t>C,D,E</t>
+  </si>
+  <si>
+    <t>C,D,E,F,G</t>
+  </si>
+  <si>
+    <t>take(i) from
+Cmaj asc</t>
+  </si>
+  <si>
+    <t>drop(i) from
+Cmaj asc</t>
+  </si>
+  <si>
+    <t>take (i-5) from
+Cmaj asc</t>
+  </si>
+  <si>
+    <t>drop(i-7) from
+Cmaj asc</t>
+  </si>
+  <si>
+    <t>index = i</t>
+  </si>
+  <si>
+    <t>take(i-7) from
+Cmaj asc</t>
+  </si>
+  <si>
+    <t>drop (i+2) from
+Cmaj asc</t>
+  </si>
 </sst>
 </file>
 
@@ -273,7 +370,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="42">
     <border>
       <left/>
       <right/>
@@ -533,13 +630,349 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -567,6 +1000,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
@@ -610,6 +1044,93 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1511,8 +2032,8 @@
       <xdr:rowOff>55221</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>681379</xdr:colOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>55880</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>3868</xdr:rowOff>
     </xdr:to>
@@ -6581,8 +7102,8 @@
       <xdr:rowOff>22087</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>662055</xdr:colOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>36556</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>169517</xdr:rowOff>
     </xdr:to>
@@ -9138,8 +9659,8 @@
       <xdr:rowOff>99392</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>639970</xdr:colOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>14471</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>6627</xdr:rowOff>
     </xdr:to>
@@ -9182,8 +9703,8 @@
       <xdr:rowOff>33130</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>31</xdr:col>
-      <xdr:colOff>736601</xdr:colOff>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>111102</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>117060</xdr:rowOff>
     </xdr:to>
@@ -11739,8 +12260,8 @@
       <xdr:rowOff>53880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>24</xdr:col>
-      <xdr:colOff>442962</xdr:colOff>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>28660</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>120073</xdr:rowOff>
     </xdr:to>
@@ -11784,7 +12305,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>321732</xdr:colOff>
+      <xdr:colOff>297084</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>145857</xdr:rowOff>
     </xdr:to>
@@ -12179,10 +12700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64D8E0F2-CA15-4242-A54E-C98928350AA8}">
-  <dimension ref="B1:AH55"/>
+  <dimension ref="B1:AH85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M39" zoomScale="139" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q58" sqref="Q58"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="P63" zoomScale="125" zoomScaleNormal="139" workbookViewId="0">
+      <selection activeCell="AC66" sqref="AC66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -12192,44 +12713,49 @@
     <col min="8" max="8" width="13.83203125" customWidth="1"/>
     <col min="10" max="10" width="10.83203125" customWidth="1"/>
     <col min="11" max="11" width="12.83203125" customWidth="1"/>
-    <col min="22" max="23" width="10.83203125" customWidth="1"/>
+    <col min="19" max="19" width="12.6640625" customWidth="1"/>
+    <col min="21" max="21" width="11.33203125" customWidth="1"/>
+    <col min="22" max="22" width="1.6640625" customWidth="1"/>
+    <col min="23" max="23" width="12.1640625" customWidth="1"/>
+    <col min="26" max="26" width="2" customWidth="1"/>
+    <col min="27" max="27" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:34" ht="17" thickBot="1"/>
     <row r="2" spans="2:34">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="F2" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="H2" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="7" t="s">
+      <c r="I2" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="9" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="2:34">
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="3"/>
       <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
@@ -12248,36 +12774,36 @@
       <c r="I3" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="2:34" ht="17" thickBot="1">
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="10">
+      <c r="C4" s="11">
         <v>0</v>
       </c>
-      <c r="D4" s="11">
+      <c r="D4" s="12">
         <v>1</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="12">
         <v>2</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="12">
         <v>3</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="12">
         <v>4</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="12">
         <v>5</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="12">
         <v>6</v>
       </c>
-      <c r="J4" s="12">
+      <c r="J4" s="13">
         <v>7</v>
       </c>
     </row>
@@ -12287,39 +12813,39 @@
       </c>
     </row>
     <row r="6" spans="2:34">
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="7" t="s">
+      <c r="E6" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="H6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="8" t="s">
+      <c r="J6" s="9" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="2:34">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="2"/>
+      <c r="C7" s="3"/>
       <c r="D7" s="1" t="s">
         <v>18</v>
       </c>
@@ -12338,74 +12864,74 @@
       <c r="I7" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="2:34" ht="17" thickBot="1">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="10">
+      <c r="C8" s="11">
         <v>0</v>
       </c>
-      <c r="D8" s="11">
+      <c r="D8" s="12">
         <v>1</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="12">
         <v>2</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="12">
         <v>3</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="12">
         <v>4</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="12">
         <v>5</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="12">
         <v>6</v>
       </c>
-      <c r="J8" s="12">
+      <c r="J8" s="13">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="2:34" ht="17" thickBot="1"/>
     <row r="10" spans="2:34">
-      <c r="K10" s="3" t="s">
+      <c r="K10" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="L10" s="6" t="s">
+      <c r="L10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="M10" s="7" t="s">
+      <c r="M10" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="N10" s="7" t="s">
+      <c r="N10" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="O10" s="7" t="s">
+      <c r="O10" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="P10" s="7" t="s">
+      <c r="P10" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="Q10" s="7" t="s">
+      <c r="Q10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="R10" s="7" t="s">
+      <c r="R10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="S10" s="8" t="s">
+      <c r="S10" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:34">
-      <c r="K11" s="4" t="s">
+      <c r="K11" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="L11" s="2" t="s">
+      <c r="L11" s="3" t="s">
         <v>0</v>
       </c>
       <c r="M11" s="1" t="s">
@@ -12426,36 +12952,36 @@
       <c r="R11" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="S11" s="9" t="s">
+      <c r="S11" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="2:34" ht="17" thickBot="1">
-      <c r="K12" s="5" t="s">
+      <c r="K12" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="L12" s="10">
+      <c r="L12" s="11">
         <v>0</v>
       </c>
-      <c r="M12" s="11">
+      <c r="M12" s="12">
         <v>1</v>
       </c>
-      <c r="N12" s="11">
+      <c r="N12" s="12">
         <v>2</v>
       </c>
-      <c r="O12" s="11">
+      <c r="O12" s="12">
         <v>3</v>
       </c>
-      <c r="P12" s="11">
+      <c r="P12" s="12">
         <v>4</v>
       </c>
-      <c r="Q12" s="11">
+      <c r="Q12" s="12">
         <v>5</v>
       </c>
-      <c r="R12" s="11">
+      <c r="R12" s="12">
         <v>6</v>
       </c>
-      <c r="S12" s="12">
+      <c r="S12" s="13">
         <v>7</v>
       </c>
     </row>
@@ -12465,119 +12991,119 @@
       </c>
     </row>
     <row r="14" spans="2:34">
-      <c r="K14" s="24" t="s">
+      <c r="K14" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="L14" s="25" t="s">
+      <c r="L14" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="M14" s="26" t="s">
+      <c r="M14" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="N14" s="26" t="s">
+      <c r="N14" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="O14" s="26" t="s">
+      <c r="O14" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="P14" s="26" t="s">
+      <c r="P14" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="Q14" s="26" t="s">
+      <c r="Q14" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="R14" s="26" t="s">
+      <c r="R14" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="S14" s="27" t="s">
+      <c r="S14" s="29" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" spans="2:34">
-      <c r="K15" s="35" t="s">
+      <c r="K15" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="L15" s="34" t="s">
+      <c r="L15" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="M15" s="28" t="s">
+      <c r="M15" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="N15" s="28" t="s">
+      <c r="N15" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="O15" s="28" t="s">
+      <c r="O15" s="30" t="s">
         <v>19</v>
       </c>
-      <c r="P15" s="28" t="s">
+      <c r="P15" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="Q15" s="28" t="s">
+      <c r="Q15" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="R15" s="28" t="s">
+      <c r="R15" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="S15" s="33" t="s">
+      <c r="S15" s="35" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="2:34" ht="17" thickBot="1">
-      <c r="K16" s="29" t="s">
+      <c r="K16" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="L16" s="30">
+      <c r="L16" s="32">
         <v>0</v>
       </c>
-      <c r="M16" s="31">
+      <c r="M16" s="33">
         <v>1</v>
       </c>
-      <c r="N16" s="31">
+      <c r="N16" s="33">
         <v>2</v>
       </c>
-      <c r="O16" s="31">
+      <c r="O16" s="33">
         <v>3</v>
       </c>
-      <c r="P16" s="31">
+      <c r="P16" s="33">
         <v>4</v>
       </c>
-      <c r="Q16" s="31">
+      <c r="Q16" s="33">
         <v>5</v>
       </c>
-      <c r="R16" s="31">
+      <c r="R16" s="33">
         <v>6</v>
       </c>
-      <c r="S16" s="32">
+      <c r="S16" s="34">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="2:34" ht="17" thickBot="1"/>
     <row r="19" spans="2:34" ht="17" thickBot="1">
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="20" t="s">
+      <c r="E19" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="21" t="s">
+      <c r="F19" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="17" t="s">
+      <c r="G19" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="18" t="s">
+      <c r="H19" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="20" spans="2:34" ht="18">
-      <c r="C20" s="16"/>
-      <c r="F20" s="16"/>
+      <c r="C20" s="17"/>
+      <c r="F20" s="17"/>
     </row>
     <row r="21" spans="2:34">
       <c r="AH21" t="s">
@@ -12586,31 +13112,31 @@
     </row>
     <row r="24" spans="2:34" ht="17" thickBot="1"/>
     <row r="25" spans="2:34" ht="17" thickBot="1">
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="D25" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="F25" s="14" t="s">
+      <c r="F25" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="G25" s="14" t="s">
+      <c r="G25" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="H25" s="15" t="s">
+      <c r="H25" s="16" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="26" spans="2:34" ht="18">
-      <c r="C26" s="16"/>
-      <c r="F26" s="16"/>
+      <c r="C26" s="17"/>
+      <c r="F26" s="17"/>
     </row>
     <row r="29" spans="2:34" ht="17" thickBot="1">
       <c r="AH29" t="s">
@@ -12618,88 +13144,88 @@
       </c>
     </row>
     <row r="30" spans="2:34" ht="17" thickBot="1">
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="D30" s="22" t="s">
+      <c r="D30" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="E30" s="20" t="s">
+      <c r="E30" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="F30" s="14" t="s">
+      <c r="F30" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="G30" s="14" t="s">
+      <c r="G30" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="H30" s="15" t="s">
+      <c r="H30" s="16" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="31" spans="2:34" ht="18">
-      <c r="C31" s="16"/>
-      <c r="F31" s="16"/>
+      <c r="C31" s="17"/>
+      <c r="F31" s="17"/>
     </row>
     <row r="35" spans="2:10" ht="17" thickBot="1"/>
     <row r="36" spans="2:10" ht="17" thickBot="1">
-      <c r="C36" s="45" t="s">
+      <c r="C36" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="E36" s="36"/>
-      <c r="H36" s="45" t="s">
+      <c r="E36" s="38"/>
+      <c r="H36" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="J36" s="36"/>
+      <c r="J36" s="38"/>
     </row>
     <row r="37" spans="2:10" ht="19" customHeight="1" thickBot="1">
-      <c r="B37" s="40" t="s">
+      <c r="B37" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="43" t="s">
+      <c r="C37" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="D37" s="42" t="s">
+      <c r="D37" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="G37" s="40"/>
-      <c r="H37" s="40" t="s">
+      <c r="E37" s="43"/>
+      <c r="G37" s="42"/>
+      <c r="H37" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="I37" s="43" t="s">
+      <c r="I37" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="J37" s="42" t="s">
+      <c r="J37" s="44" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="38" spans="2:10">
-      <c r="B38" s="38" t="s">
+      <c r="B38" s="40" t="s">
         <v>33</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D38" s="37" t="s">
+      <c r="D38" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="E38" s="38" t="s">
+      <c r="E38" s="40" t="s">
         <v>44</v>
       </c>
-      <c r="G38" s="38" t="s">
+      <c r="G38" s="40" t="s">
         <v>33</v>
       </c>
-      <c r="H38" s="38" t="s">
+      <c r="H38" s="40" t="s">
         <v>35</v>
       </c>
-      <c r="I38" s="44" t="s">
+      <c r="I38" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="J38" s="39" t="s">
+      <c r="J38" s="41" t="s">
         <v>40</v>
       </c>
     </row>
@@ -12710,7 +13236,7 @@
       <c r="C39" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D39" s="37" t="s">
+      <c r="D39" s="39" t="s">
         <v>5</v>
       </c>
       <c r="E39" s="1" t="s">
@@ -12722,10 +13248,10 @@
       <c r="H39" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I39" s="23" t="s">
+      <c r="I39" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="J39" s="37" t="s">
+      <c r="J39" s="39" t="s">
         <v>43</v>
       </c>
     </row>
@@ -12733,10 +13259,10 @@
       <c r="B40" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="38" t="s">
+      <c r="C40" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="D40" s="39" t="s">
+      <c r="D40" s="41" t="s">
         <v>41</v>
       </c>
       <c r="E40" s="1"/>
@@ -12746,7 +13272,7 @@
       <c r="H40" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I40" s="23" t="s">
+      <c r="I40" s="25" t="s">
         <v>4</v>
       </c>
       <c r="J40" s="1" t="s">
@@ -12760,7 +13286,7 @@
       <c r="C41" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D41" s="37" t="s">
+      <c r="D41" s="39" t="s">
         <v>39</v>
       </c>
       <c r="E41" s="1"/>
@@ -12768,7 +13294,7 @@
       <c r="H41" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I41" s="23" t="s">
+      <c r="I41" s="25" t="s">
         <v>5</v>
       </c>
       <c r="J41" s="1" t="s">
@@ -12782,7 +13308,7 @@
       <c r="C42" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D42" s="37" t="s">
+      <c r="D42" s="39" t="s">
         <v>42</v>
       </c>
       <c r="E42" s="1"/>
@@ -12790,7 +13316,7 @@
       <c r="H42" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I42" s="37" t="s">
+      <c r="I42" s="39" t="s">
         <v>41</v>
       </c>
       <c r="J42" s="1"/>
@@ -12800,15 +13326,15 @@
       <c r="C43" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="37" t="s">
+      <c r="D43" s="39" t="s">
         <v>40</v>
       </c>
       <c r="E43" s="1"/>
       <c r="G43" s="1"/>
-      <c r="H43" s="23" t="s">
+      <c r="H43" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="I43" s="37" t="s">
+      <c r="I43" s="39" t="s">
         <v>39</v>
       </c>
       <c r="J43" s="1"/>
@@ -12818,89 +13344,89 @@
       <c r="C44" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D44" s="37" t="s">
+      <c r="D44" s="39" t="s">
         <v>43</v>
       </c>
       <c r="E44" s="1"/>
       <c r="G44" s="1"/>
-      <c r="H44" s="23" t="s">
+      <c r="H44" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="I44" s="37" t="s">
+      <c r="I44" s="39" t="s">
         <v>42</v>
       </c>
       <c r="J44" s="1"/>
     </row>
     <row r="45" spans="2:10" ht="17" thickBot="1"/>
     <row r="46" spans="2:10" ht="17" thickBot="1">
-      <c r="C46" s="45" t="s">
+      <c r="C46" s="47" t="s">
         <v>48</v>
       </c>
-      <c r="E46" s="36"/>
-      <c r="H46" s="45" t="s">
+      <c r="E46" s="38"/>
+      <c r="H46" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="J46" s="36"/>
+      <c r="J46" s="38"/>
     </row>
     <row r="47" spans="2:10" ht="20" customHeight="1" thickBot="1">
-      <c r="B47" s="40" t="s">
+      <c r="B47" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="C47" s="43" t="s">
+      <c r="C47" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="D47" s="42" t="s">
+      <c r="D47" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="E47" s="41"/>
-      <c r="G47" s="40"/>
-      <c r="H47" s="40" t="s">
+      <c r="E47" s="43"/>
+      <c r="G47" s="42"/>
+      <c r="H47" s="42" t="s">
         <v>31</v>
       </c>
-      <c r="I47" s="43" t="s">
+      <c r="I47" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="J47" s="42" t="s">
+      <c r="J47" s="44" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="48" spans="2:10">
-      <c r="B48" s="38" t="s">
+      <c r="B48" s="40" t="s">
         <v>33</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D48" s="37" t="s">
+      <c r="D48" s="39" t="s">
         <v>3</v>
       </c>
-      <c r="E48" s="38" t="s">
+      <c r="E48" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="G48" s="38" t="s">
+      <c r="G48" s="40" t="s">
         <v>33</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I48" s="39" t="s">
+      <c r="I48" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="J48" s="37" t="s">
+      <c r="J48" s="39" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="49" spans="2:19">
+    <row r="49" spans="2:21">
       <c r="B49" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D49" s="37" t="s">
+      <c r="D49" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="E49" s="38" t="s">
+      <c r="E49" s="40" t="s">
         <v>44</v>
       </c>
       <c r="G49" s="1" t="s">
@@ -12909,14 +13435,14 @@
       <c r="H49" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I49" s="37" t="s">
+      <c r="I49" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="J49" s="37" t="s">
+      <c r="J49" s="39" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="2:19">
+    <row r="50" spans="2:21">
       <c r="B50" s="1" t="s">
         <v>34</v>
       </c>
@@ -12936,18 +13462,18 @@
       <c r="I50" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J50" s="37" t="s">
+      <c r="J50" s="39" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="51" spans="2:19">
+    <row r="51" spans="2:21">
       <c r="B51" s="1" t="s">
         <v>35</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D51" s="37" t="s">
+      <c r="D51" s="39" t="s">
         <v>41</v>
       </c>
       <c r="E51" s="1"/>
@@ -12958,16 +13484,16 @@
       <c r="I51" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J51" s="38" t="s">
+      <c r="J51" s="40" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="52" spans="2:19">
+    <row r="52" spans="2:21">
       <c r="B52" s="1"/>
       <c r="C52" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D52" s="37" t="s">
+      <c r="D52" s="39" t="s">
         <v>39</v>
       </c>
       <c r="E52" s="1"/>
@@ -12982,12 +13508,12 @@
         <v>45</v>
       </c>
     </row>
-    <row r="53" spans="2:19">
+    <row r="53" spans="2:21">
       <c r="B53" s="1"/>
       <c r="C53" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D53" s="37" t="s">
+      <c r="D53" s="39" t="s">
         <v>42</v>
       </c>
       <c r="E53" s="1"/>
@@ -12995,17 +13521,17 @@
       <c r="H53" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I53" s="39" t="s">
+      <c r="I53" s="41" t="s">
         <v>41</v>
       </c>
       <c r="J53" s="1"/>
     </row>
-    <row r="54" spans="2:19">
+    <row r="54" spans="2:21">
       <c r="B54" s="1"/>
       <c r="C54" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D54" s="37" t="s">
+      <c r="D54" s="39" t="s">
         <v>40</v>
       </c>
       <c r="E54" s="1"/>
@@ -13013,16 +13539,397 @@
       <c r="H54" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="I54" s="37" t="s">
+      <c r="I54" s="39" t="s">
         <v>39</v>
       </c>
       <c r="J54" s="1"/>
-      <c r="R54" s="47"/>
-      <c r="S54" s="47"/>
+      <c r="R54" s="49"/>
+      <c r="S54" s="49"/>
     </row>
-    <row r="55" spans="2:19">
-      <c r="C55" s="46"/>
-      <c r="R55" s="47"/>
+    <row r="55" spans="2:21">
+      <c r="C55" s="48"/>
+      <c r="R55" s="49"/>
+    </row>
+    <row r="59" spans="2:21" ht="17" thickBot="1"/>
+    <row r="60" spans="2:21" ht="17" thickBot="1">
+      <c r="N60" t="s">
+        <v>65</v>
+      </c>
+      <c r="O60" s="48"/>
+      <c r="P60" s="76" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q60" s="77" t="s">
+        <v>54</v>
+      </c>
+      <c r="R60" s="78" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="61" spans="2:21" ht="34">
+      <c r="O61" s="74" t="s">
+        <v>0</v>
+      </c>
+      <c r="P61" s="79" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q61" s="80" t="s">
+        <v>57</v>
+      </c>
+      <c r="R61" s="81"/>
+    </row>
+    <row r="62" spans="2:21" ht="34">
+      <c r="O62" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="P62" s="82" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q62" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="R62" s="83"/>
+    </row>
+    <row r="63" spans="2:21" ht="34">
+      <c r="O63" s="24" t="s">
+        <v>4</v>
+      </c>
+      <c r="P63" s="82" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q63" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="R63" s="83"/>
+    </row>
+    <row r="64" spans="2:21" ht="34">
+      <c r="O64" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="P64" s="82" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q64" s="2">
+        <v>12</v>
+      </c>
+      <c r="R64" s="83">
+        <v>1</v>
+      </c>
+      <c r="U64" s="48"/>
+    </row>
+    <row r="65" spans="15:29" ht="34">
+      <c r="O65" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="P65" s="82" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q65" s="2">
+        <v>12</v>
+      </c>
+      <c r="R65" s="83">
+        <v>1</v>
+      </c>
+      <c r="U65" s="48"/>
+    </row>
+    <row r="66" spans="15:29" ht="34">
+      <c r="O66" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="P66" s="82" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q66" s="2"/>
+      <c r="R66" s="83" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="15:29" ht="35" thickBot="1">
+      <c r="O67" s="75" t="s">
+        <v>5</v>
+      </c>
+      <c r="P67" s="84" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q67" s="85"/>
+      <c r="R67" s="86" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="68" spans="15:29" ht="17" thickBot="1"/>
+    <row r="69" spans="15:29" ht="17" thickBot="1">
+      <c r="T69" s="48"/>
+      <c r="U69" s="64" t="s">
+        <v>53</v>
+      </c>
+      <c r="X69" s="48"/>
+      <c r="Y69" s="64" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB69" s="48"/>
+      <c r="AC69" s="64" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="70" spans="15:29" ht="17" thickBot="1">
+      <c r="T70" s="63"/>
+      <c r="V70" s="63"/>
+      <c r="X70" s="63"/>
+      <c r="Z70" s="63"/>
+      <c r="AB70" s="63"/>
+    </row>
+    <row r="71" spans="15:29" ht="17" customHeight="1" thickBot="1">
+      <c r="T71" s="64" t="s">
+        <v>78</v>
+      </c>
+      <c r="U71" s="65"/>
+      <c r="V71" s="63"/>
+      <c r="X71" s="64" t="s">
+        <v>78</v>
+      </c>
+      <c r="Y71" s="65"/>
+      <c r="Z71" s="63"/>
+      <c r="AB71" s="64" t="s">
+        <v>78</v>
+      </c>
+      <c r="AC71" s="65"/>
+    </row>
+    <row r="72" spans="15:29" ht="32" customHeight="1">
+      <c r="S72" s="87" t="s">
+        <v>74</v>
+      </c>
+      <c r="T72" s="66">
+        <v>2</v>
+      </c>
+      <c r="U72" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="V72" s="63"/>
+      <c r="W72" s="87" t="s">
+        <v>79</v>
+      </c>
+      <c r="X72" s="66">
+        <v>8</v>
+      </c>
+      <c r="Y72" s="54" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z72" s="63"/>
+      <c r="AA72" s="87" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB72" s="66">
+        <v>1</v>
+      </c>
+      <c r="AC72" s="57" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="15:29" ht="18" thickBot="1">
+      <c r="S73" s="88"/>
+      <c r="T73" s="67">
+        <v>4</v>
+      </c>
+      <c r="U73" s="55" t="s">
+        <v>67</v>
+      </c>
+      <c r="V73" s="63"/>
+      <c r="W73" s="88"/>
+      <c r="X73" s="67">
+        <v>10</v>
+      </c>
+      <c r="Y73" s="55" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z73" s="63"/>
+      <c r="AB73" s="68">
+        <v>3</v>
+      </c>
+      <c r="AC73" s="59" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="74" spans="15:29" ht="18" thickBot="1">
+      <c r="S74" s="88"/>
+      <c r="T74" s="68">
+        <v>6</v>
+      </c>
+      <c r="U74" s="56" t="s">
+        <v>68</v>
+      </c>
+      <c r="V74" s="63"/>
+      <c r="W74" s="88"/>
+      <c r="X74" s="68">
+        <v>12</v>
+      </c>
+      <c r="Y74" s="56" t="s">
+        <v>73</v>
+      </c>
+      <c r="Z74" s="63"/>
+      <c r="AA74" s="65"/>
+      <c r="AB74" s="50"/>
+    </row>
+    <row r="75" spans="15:29" ht="4" customHeight="1" thickBot="1">
+      <c r="S75" s="88"/>
+      <c r="T75" s="63"/>
+      <c r="U75" s="63"/>
+      <c r="V75" s="63"/>
+      <c r="W75" s="88"/>
+      <c r="X75" s="63"/>
+      <c r="Y75" s="63"/>
+      <c r="Z75" s="63"/>
+      <c r="AA75" s="53"/>
+      <c r="AB75" s="63"/>
+    </row>
+    <row r="76" spans="15:29" ht="36" customHeight="1" thickBot="1">
+      <c r="S76" s="87" t="s">
+        <v>77</v>
+      </c>
+      <c r="T76" s="66">
+        <v>8</v>
+      </c>
+      <c r="U76" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="V76" s="63"/>
+      <c r="W76" s="87" t="s">
+        <v>74</v>
+      </c>
+      <c r="X76" s="69">
+        <v>13</v>
+      </c>
+      <c r="Y76" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z76" s="63"/>
+      <c r="AA76" s="53"/>
+      <c r="AB76" s="63"/>
+    </row>
+    <row r="77" spans="15:29" ht="17">
+      <c r="S77" s="88"/>
+      <c r="T77" s="67">
+        <v>10</v>
+      </c>
+      <c r="U77" s="58" t="s">
+        <v>70</v>
+      </c>
+      <c r="V77" s="63"/>
+      <c r="W77" s="65"/>
+      <c r="X77" s="51"/>
+      <c r="Y77" s="63"/>
+      <c r="Z77" s="63"/>
+      <c r="AA77" s="63"/>
+    </row>
+    <row r="78" spans="15:29" ht="18" thickBot="1">
+      <c r="S78" s="88"/>
+      <c r="T78" s="68">
+        <v>12</v>
+      </c>
+      <c r="U78" s="59" t="s">
+        <v>71</v>
+      </c>
+      <c r="V78" s="63"/>
+      <c r="W78" s="65"/>
+      <c r="X78" s="51"/>
+      <c r="Y78" s="63"/>
+      <c r="Z78" s="63"/>
+      <c r="AA78" s="63"/>
+    </row>
+    <row r="79" spans="15:29" ht="4" customHeight="1" thickBot="1">
+      <c r="S79" s="88"/>
+      <c r="T79" s="63"/>
+      <c r="U79" s="63"/>
+      <c r="V79" s="63"/>
+      <c r="W79" s="65"/>
+      <c r="X79" s="65"/>
+      <c r="Y79" s="63"/>
+      <c r="Z79" s="63"/>
+      <c r="AA79" s="63"/>
+    </row>
+    <row r="80" spans="15:29" ht="51">
+      <c r="S80" s="87" t="s">
+        <v>76</v>
+      </c>
+      <c r="T80" s="66">
+        <v>7</v>
+      </c>
+      <c r="U80" s="54" t="s">
+        <v>66</v>
+      </c>
+      <c r="V80" s="63"/>
+      <c r="W80" s="65"/>
+      <c r="X80" s="50"/>
+      <c r="Y80" s="63"/>
+      <c r="Z80" s="63"/>
+      <c r="AA80" s="63"/>
+    </row>
+    <row r="81" spans="19:27" ht="17">
+      <c r="S81" s="88"/>
+      <c r="T81" s="70">
+        <v>9</v>
+      </c>
+      <c r="U81" s="60" t="s">
+        <v>67</v>
+      </c>
+      <c r="V81" s="63"/>
+      <c r="W81" s="71"/>
+      <c r="X81" s="52"/>
+      <c r="Y81" s="63"/>
+      <c r="Z81" s="63"/>
+      <c r="AA81" s="63"/>
+    </row>
+    <row r="82" spans="19:27" ht="18" thickBot="1">
+      <c r="S82" s="88"/>
+      <c r="T82" s="72">
+        <v>11</v>
+      </c>
+      <c r="U82" s="61" t="s">
+        <v>68</v>
+      </c>
+      <c r="V82" s="63"/>
+      <c r="W82" s="71"/>
+      <c r="X82" s="52"/>
+      <c r="Y82" s="63"/>
+      <c r="Z82" s="63"/>
+      <c r="AA82" s="63"/>
+    </row>
+    <row r="83" spans="19:27" ht="4" customHeight="1" thickBot="1">
+      <c r="S83" s="88"/>
+      <c r="T83" s="65"/>
+      <c r="U83" s="65"/>
+      <c r="V83" s="63"/>
+      <c r="W83" s="63"/>
+      <c r="X83" s="63"/>
+      <c r="Y83" s="63"/>
+      <c r="Z83" s="63"/>
+      <c r="AA83" s="63"/>
+    </row>
+    <row r="84" spans="19:27" ht="35" thickBot="1">
+      <c r="S84" s="87" t="s">
+        <v>75</v>
+      </c>
+      <c r="T84" s="69">
+        <v>13</v>
+      </c>
+      <c r="U84" s="73" t="s">
+        <v>69</v>
+      </c>
+      <c r="V84" s="63"/>
+      <c r="W84" s="63"/>
+      <c r="X84" s="63"/>
+      <c r="Y84" s="63"/>
+      <c r="Z84" s="63"/>
+      <c r="AA84" s="63"/>
+    </row>
+    <row r="85" spans="19:27">
+      <c r="T85" s="63"/>
+      <c r="U85" s="63"/>
+      <c r="V85" s="63"/>
+      <c r="W85" s="63"/>
+      <c r="X85" s="63"/>
+      <c r="Y85" s="63"/>
+      <c r="Z85" s="63"/>
+      <c r="AA85" s="63"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
create the harmseq octave analysis diagrams in paper
</commit_message>
<xml_diff>
--- a/Paper/ir_expansion_diagrams.xlsx
+++ b/Paper/ir_expansion_diagrams.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ilanashapiro/Documents/CS132/MusAssist/Paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3D6AD74-7FA3-D944-8A93-5B1EC2B38314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E71A4008-38F1-5E40-A363-D37FB8C4DDE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{9CC0B3E8-72D6-5245-A968-31A972243904}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="109">
   <si>
     <t>C</t>
   </si>
@@ -217,7 +217,16 @@
 7,9,11,13</t>
   </si>
   <si>
+    <t>7,9,11,13</t>
+  </si>
+  <si>
     <t>10,12</t>
+  </si>
+  <si>
+    <t>9,11,13</t>
+  </si>
+  <si>
+    <t>11,13</t>
   </si>
   <si>
     <t>1,3</t>
@@ -270,10 +279,6 @@
 Cmaj asc</t>
   </si>
   <si>
-    <t>drop(i) from
-Cmaj asc</t>
-  </si>
-  <si>
     <t>take (i-5) from
 Cmaj asc</t>
   </si>
@@ -291,6 +296,102 @@
   <si>
     <t>drop (i+2) from
 Cmaj asc</t>
+  </si>
+  <si>
+    <t>Asc Fifths</t>
+  </si>
+  <si>
+    <t>succ2</t>
+  </si>
+  <si>
+    <t>12
+5,7,9,11,13</t>
+  </si>
+  <si>
+    <t>10,12
+3,5,7,9,11,13</t>
+  </si>
+  <si>
+    <t>8,10,12
+1,3,5,7,9,11,13</t>
+  </si>
+  <si>
+    <t>6,8,10,12
+1,3,5,7,9,11</t>
+  </si>
+  <si>
+    <t>4,6,8,10,12
+1,3,5,7,9</t>
+  </si>
+  <si>
+    <t>2,4,6,8,10,12
+1,3,5,7</t>
+  </si>
+  <si>
+    <t>G,A,B</t>
+  </si>
+  <si>
+    <t>E,F,G,A,B</t>
+  </si>
+  <si>
+    <t>C,D,E,F,G,A,B</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> take(             )      
+from Cmaj desc</t>
+  </si>
+  <si>
+    <t>Asc 5-6</t>
+  </si>
+  <si>
+    <t>4,6,8,10,12
+9,11,13</t>
+  </si>
+  <si>
+    <t>2,4,6,8,10,12
+7,9,11,13</t>
+  </si>
+  <si>
+    <t>special cases</t>
+  </si>
+  <si>
+    <t>take(         ) from
+Cmaj desc</t>
+  </si>
+  <si>
+    <t>drop(1) from
+Cmaj asc</t>
+  </si>
+  <si>
+    <t>take(1) from
+Cmaj asc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> take(         )      
+from Cmaj desc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> take(         )      
+from Cmaj asc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> take(        )      
+from Cmaj desc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> take(        )      
+from Cmaj asc</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> take(   )      
+from Cmaj asc</t>
+  </si>
+  <si>
+    <t>Desc Fifths</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> drop(        )      
+from Cmaj asc</t>
   </si>
 </sst>
 </file>
@@ -370,7 +471,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="46">
     <border>
       <left/>
       <right/>
@@ -780,6 +881,32 @@
     </border>
     <border>
       <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
         <color indexed="64"/>
       </left>
       <right/>
@@ -963,12 +1090,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color theme="1"/>
+      </right>
+      <top style="medium">
+        <color theme="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="107">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1093,22 +1249,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -1123,6 +1274,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1130,6 +1287,46 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2032,8 +2229,8 @@
       <xdr:rowOff>55221</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>55880</xdr:colOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>649660</xdr:colOff>
       <xdr:row>6</xdr:row>
       <xdr:rowOff>3868</xdr:rowOff>
     </xdr:to>
@@ -7102,8 +7299,8 @@
       <xdr:rowOff>22087</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>36556</xdr:colOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>632109</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>169517</xdr:rowOff>
     </xdr:to>
@@ -9659,8 +9856,8 @@
       <xdr:rowOff>99392</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>14471</xdr:colOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>610024</xdr:colOff>
       <xdr:row>22</xdr:row>
       <xdr:rowOff>6627</xdr:rowOff>
     </xdr:to>
@@ -9703,8 +9900,8 @@
       <xdr:rowOff>33130</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>111102</xdr:colOff>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>704570</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>117060</xdr:rowOff>
     </xdr:to>
@@ -12260,8 +12457,8 @@
       <xdr:rowOff>53880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>25</xdr:col>
-      <xdr:colOff>28660</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>241783</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>120073</xdr:rowOff>
     </xdr:to>
@@ -12305,7 +12502,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>297084</xdr:colOff>
+      <xdr:colOff>297085</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>145857</xdr:rowOff>
     </xdr:to>
@@ -12400,6 +12597,1743 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>579766</xdr:colOff>
+      <xdr:row>103</xdr:row>
+      <xdr:rowOff>24328</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="366703" cy="306762"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="246" name="TextBox 245">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C3088F1-BAC9-184C-8A03-1506A70365AC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="16512493" y="25395464"/>
+              <a:ext cx="366703" cy="306762"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:f>
+                    <m:fPr>
+                      <m:ctrlPr>
+                        <a:rPr lang="en-US" sz="1200" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                      </m:ctrlPr>
+                    </m:fPr>
+                    <m:num>
+                      <m:r>
+                        <m:rPr>
+                          <m:sty m:val="p"/>
+                        </m:rPr>
+                        <a:rPr lang="en-US" sz="1200" b="0" i="0">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>i</m:t>
+                      </m:r>
+                      <m:r>
+                        <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>−1</m:t>
+                      </m:r>
+                    </m:num>
+                    <m:den>
+                      <m:r>
+                        <a:rPr lang="en-US" sz="1200" b="0" i="1">
+                          <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                        </a:rPr>
+                        <m:t>2</m:t>
+                      </m:r>
+                    </m:den>
+                  </m:f>
+                </m:oMath>
+              </a14:m>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>+4</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="246" name="TextBox 245">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C3088F1-BAC9-184C-8A03-1506A70365AC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="16512493" y="25395464"/>
+              <a:ext cx="366703" cy="306762"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1200" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>i−1)/2</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+                </a:rPr>
+                <a:t>+4</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>583060</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>10131</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="451864" cy="306762"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="247" name="TextBox 246">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27536FBF-19D7-9B40-8E1A-8278558721A4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="16587213" y="26992250"/>
+              <a:ext cx="451864" cy="306762"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="900" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <m:rPr>
+                            <m:sty m:val="p"/>
+                          </m:rPr>
+                          <a:rPr lang="en-US" sz="900" b="0" i="0">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>i</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="900" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−7</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="900" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="800">
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="247" name="TextBox 246">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27536FBF-19D7-9B40-8E1A-8278558721A4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="16587213" y="26992250"/>
+              <a:ext cx="451864" cy="306762"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>i−7)/2</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="800">
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>570651</xdr:colOff>
+      <xdr:row>96</xdr:row>
+      <xdr:rowOff>186111</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="451864" cy="306762"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="248" name="TextBox 247">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60E5EE35-3A43-E349-A5BF-EEC7E8128FD6}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="19353662" y="23832645"/>
+              <a:ext cx="451864" cy="306762"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="900" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <m:rPr>
+                            <m:sty m:val="p"/>
+                          </m:rPr>
+                          <a:rPr lang="en-US" sz="900" b="0" i="0">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>i</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="900" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−7</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="900" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="800">
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="248" name="TextBox 247">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{60E5EE35-3A43-E349-A5BF-EEC7E8128FD6}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="19353662" y="23832645"/>
+              <a:ext cx="451864" cy="306762"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>i−7)/2</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="800">
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>664042</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>1614</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="366703" cy="306762"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="254" name="TextBox 253">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23836744-C6CD-7147-A27E-19561CD93984}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="19430805" y="33871326"/>
+              <a:ext cx="366703" cy="306762"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="900" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <m:rPr>
+                            <m:sty m:val="p"/>
+                          </m:rPr>
+                          <a:rPr lang="en-US" sz="900" b="0" i="0">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>i</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="900" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−5</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="900" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="800">
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="254" name="TextBox 253">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23836744-C6CD-7147-A27E-19561CD93984}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="19430805" y="33871326"/>
+              <a:ext cx="366703" cy="306762"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>i−5)/2</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="800">
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>580158</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>5112</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="451864" cy="306762"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="256" name="TextBox 255">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71F9D1AE-8C38-3441-A602-A963B7062CA0}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="16512885" y="23868123"/>
+              <a:ext cx="451864" cy="306762"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="800" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <m:rPr>
+                            <m:sty m:val="p"/>
+                          </m:rPr>
+                          <a:rPr lang="en-US" sz="800" b="0" i="0">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>i</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="800" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−1</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="800" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="700">
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="256" name="TextBox 255">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71F9D1AE-8C38-3441-A602-A963B7062CA0}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="16512885" y="23868123"/>
+              <a:ext cx="451864" cy="306762"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="800" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>i−1)/2</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="700">
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>649020</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>40792</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="366703" cy="306762"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="257" name="TextBox 256">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10064BD1-45AF-794D-B01B-257AA452A2B7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="19415783" y="32110576"/>
+              <a:ext cx="366703" cy="306762"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="900" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <m:rPr>
+                            <m:sty m:val="p"/>
+                          </m:rPr>
+                          <a:rPr lang="en-US" sz="900" b="0" i="0">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>i</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="900" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−1</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="900" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="800">
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="257" name="TextBox 256">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{10064BD1-45AF-794D-B01B-257AA452A2B7}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="19415783" y="32110576"/>
+              <a:ext cx="366703" cy="306762"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>i−1)/2</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="800">
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>673179</xdr:colOff>
+      <xdr:row>165</xdr:row>
+      <xdr:rowOff>19887</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="366703" cy="306762"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="258" name="TextBox 257">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C32A42DA-D848-2443-8293-60EE5F5AEC00}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="19439942" y="42514635"/>
+              <a:ext cx="366703" cy="306762"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="900" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <m:rPr>
+                            <m:sty m:val="p"/>
+                          </m:rPr>
+                          <a:rPr lang="en-US" sz="900" b="0" i="0">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>i</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="900" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−7</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="900" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="800">
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="258" name="TextBox 257">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C32A42DA-D848-2443-8293-60EE5F5AEC00}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="19439942" y="42514635"/>
+              <a:ext cx="366703" cy="306762"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>i−7)/2</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="800">
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>754819</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>7498</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="366703" cy="306762"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="259" name="TextBox 258">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84CA0AEF-6614-E240-B9AD-08B74E2885F4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="19521582" y="39578505"/>
+              <a:ext cx="366703" cy="306762"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="900" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <m:rPr>
+                            <m:sty m:val="p"/>
+                          </m:rPr>
+                          <a:rPr lang="en-US" sz="900" b="0" i="0">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>i</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="900" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="800">
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="259" name="TextBox 258">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84CA0AEF-6614-E240-B9AD-08B74E2885F4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="19521582" y="39578505"/>
+              <a:ext cx="366703" cy="306762"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>i/2</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="800">
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>633583</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>53181</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="366703" cy="306762"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="260" name="TextBox 259">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C9AB934-B4FC-544F-9F0B-2267167D40DF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="16566310" y="39545851"/>
+              <a:ext cx="366703" cy="306762"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="900" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <m:rPr>
+                            <m:sty m:val="p"/>
+                          </m:rPr>
+                          <a:rPr lang="en-US" sz="900" b="0" i="0">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>i</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="900" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>−7</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="900" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="800">
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="260" name="TextBox 259">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C9AB934-B4FC-544F-9F0B-2267167D40DF}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="16566310" y="39545851"/>
+              <a:ext cx="366703" cy="306762"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>i−7)/2</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="800">
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>673179</xdr:colOff>
+      <xdr:row>159</xdr:row>
+      <xdr:rowOff>202621</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="366703" cy="306762"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="261" name="TextBox 260">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98F78D54-DF8C-1842-ADDA-D9ADCA7CDE23}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="19439942" y="41852591"/>
+              <a:ext cx="366703" cy="306762"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:f>
+                      <m:fPr>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="900" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:fPr>
+                      <m:num>
+                        <m:r>
+                          <m:rPr>
+                            <m:sty m:val="p"/>
+                          </m:rPr>
+                          <a:rPr lang="en-US" sz="900" b="0" i="0">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>i</m:t>
+                        </m:r>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="900" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>+7</m:t>
+                        </m:r>
+                      </m:num>
+                      <m:den>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="900" b="0" i="1">
+                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                            <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                          </a:rPr>
+                          <m:t>2</m:t>
+                        </m:r>
+                      </m:den>
+                    </m:f>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="800">
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="261" name="TextBox 260">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98F78D54-DF8C-1842-ADDA-D9ADCA7CDE23}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="19439942" y="41852591"/>
+              <a:ext cx="366703" cy="306762"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:noAutofit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>(</a:t>
+              </a:r>
+              <a:r>
+                <a:rPr lang="en-US" sz="900" b="0" i="0">
+                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                </a:rPr>
+                <a:t>i+7)/2</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="800">
+                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:ea typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
+                <a:cs typeface="Calibri" panose="020F0502020204030204" pitchFamily="34" charset="0"/>
+              </a:endParaRPr>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -12700,10 +14634,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64D8E0F2-CA15-4242-A54E-C98928350AA8}">
-  <dimension ref="B1:AH85"/>
+  <dimension ref="B1:AH169"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="P63" zoomScale="125" zoomScaleNormal="139" workbookViewId="0">
-      <selection activeCell="AC66" sqref="AC66"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="M144" zoomScale="139" zoomScaleNormal="187" workbookViewId="0">
+      <selection activeCell="AB152" sqref="AB152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -12713,97 +14647,100 @@
     <col min="8" max="8" width="13.83203125" customWidth="1"/>
     <col min="10" max="10" width="10.83203125" customWidth="1"/>
     <col min="11" max="11" width="12.83203125" customWidth="1"/>
-    <col min="19" max="19" width="12.6640625" customWidth="1"/>
+    <col min="16" max="16" width="14.83203125" customWidth="1"/>
+    <col min="17" max="17" width="12.1640625" customWidth="1"/>
+    <col min="19" max="19" width="13.5" customWidth="1"/>
     <col min="21" max="21" width="11.33203125" customWidth="1"/>
     <col min="22" max="22" width="1.6640625" customWidth="1"/>
-    <col min="23" max="23" width="12.1640625" customWidth="1"/>
+    <col min="23" max="23" width="14" customWidth="1"/>
+    <col min="25" max="25" width="11.83203125" customWidth="1"/>
     <col min="26" max="26" width="2" customWidth="1"/>
     <col min="27" max="27" width="13.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:34" ht="17" thickBot="1"/>
     <row r="2" spans="2:34">
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="8" t="s">
+      <c r="G2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="H2" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="8" t="s">
+      <c r="I2" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="10" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="2:34">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="1" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="11" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="2:34" ht="17" thickBot="1">
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="11">
+      <c r="C4" s="12">
         <v>0</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="13">
         <v>1</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="13">
         <v>2</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="13">
         <v>3</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="13">
         <v>4</v>
       </c>
-      <c r="H4" s="12">
+      <c r="H4" s="13">
         <v>5</v>
       </c>
-      <c r="I4" s="12">
+      <c r="I4" s="13">
         <v>6</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="14">
         <v>7</v>
       </c>
     </row>
@@ -12813,175 +14750,175 @@
       </c>
     </row>
     <row r="6" spans="2:34">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="H6" s="8" t="s">
+      <c r="H6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="8" t="s">
+      <c r="I6" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="7" spans="2:34">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="1" t="s">
+      <c r="C7" s="4"/>
+      <c r="D7" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="I7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="J7" s="11" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="8" spans="2:34" ht="17" thickBot="1">
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="11">
+      <c r="C8" s="12">
         <v>0</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="13">
         <v>1</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="13">
         <v>2</v>
       </c>
-      <c r="F8" s="12">
+      <c r="F8" s="13">
         <v>3</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="13">
         <v>4</v>
       </c>
-      <c r="H8" s="12">
+      <c r="H8" s="13">
         <v>5</v>
       </c>
-      <c r="I8" s="12">
+      <c r="I8" s="13">
         <v>6</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="14">
         <v>7</v>
       </c>
     </row>
     <row r="9" spans="2:34" ht="17" thickBot="1"/>
     <row r="10" spans="2:34">
-      <c r="K10" s="4" t="s">
+      <c r="K10" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="L10" s="7" t="s">
+      <c r="L10" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="M10" s="8" t="s">
+      <c r="M10" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="N10" s="8" t="s">
+      <c r="N10" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="O10" s="8" t="s">
+      <c r="O10" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="P10" s="8" t="s">
+      <c r="P10" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="Q10" s="8" t="s">
+      <c r="Q10" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="R10" s="8" t="s">
+      <c r="R10" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="S10" s="9" t="s">
+      <c r="S10" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="2:34">
-      <c r="K11" s="5" t="s">
+      <c r="K11" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="L11" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="M11" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="N11" s="1" t="s">
+      <c r="N11" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="O11" s="1" t="s">
+      <c r="O11" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="P11" s="1" t="s">
+      <c r="P11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="Q11" s="1" t="s">
+      <c r="Q11" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="R11" s="1" t="s">
+      <c r="R11" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="S11" s="10" t="s">
+      <c r="S11" s="11" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="12" spans="2:34" ht="17" thickBot="1">
-      <c r="K12" s="6" t="s">
+      <c r="K12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="L12" s="11">
+      <c r="L12" s="12">
         <v>0</v>
       </c>
-      <c r="M12" s="12">
+      <c r="M12" s="13">
         <v>1</v>
       </c>
-      <c r="N12" s="12">
+      <c r="N12" s="13">
         <v>2</v>
       </c>
-      <c r="O12" s="12">
+      <c r="O12" s="13">
         <v>3</v>
       </c>
-      <c r="P12" s="12">
+      <c r="P12" s="13">
         <v>4</v>
       </c>
-      <c r="Q12" s="12">
+      <c r="Q12" s="13">
         <v>5</v>
       </c>
-      <c r="R12" s="12">
+      <c r="R12" s="13">
         <v>6</v>
       </c>
-      <c r="S12" s="13">
+      <c r="S12" s="14">
         <v>7</v>
       </c>
     </row>
@@ -12991,119 +14928,119 @@
       </c>
     </row>
     <row r="14" spans="2:34">
-      <c r="K14" s="26" t="s">
+      <c r="K14" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="L14" s="27" t="s">
+      <c r="L14" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="M14" s="28" t="s">
+      <c r="M14" s="29" t="s">
         <v>2</v>
       </c>
-      <c r="N14" s="28" t="s">
+      <c r="N14" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="O14" s="28" t="s">
+      <c r="O14" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="P14" s="28" t="s">
+      <c r="P14" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="Q14" s="28" t="s">
+      <c r="Q14" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="R14" s="28" t="s">
+      <c r="R14" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="S14" s="29" t="s">
+      <c r="S14" s="30" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" spans="2:34">
-      <c r="K15" s="37" t="s">
+      <c r="K15" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="L15" s="36" t="s">
+      <c r="L15" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="M15" s="30" t="s">
+      <c r="M15" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="N15" s="30" t="s">
+      <c r="N15" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="O15" s="30" t="s">
+      <c r="O15" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="P15" s="30" t="s">
+      <c r="P15" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="Q15" s="30" t="s">
+      <c r="Q15" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="R15" s="30" t="s">
+      <c r="R15" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="S15" s="35" t="s">
+      <c r="S15" s="36" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="2:34" ht="17" thickBot="1">
-      <c r="K16" s="31" t="s">
+      <c r="K16" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="L16" s="32">
+      <c r="L16" s="33">
         <v>0</v>
       </c>
-      <c r="M16" s="33">
+      <c r="M16" s="34">
         <v>1</v>
       </c>
-      <c r="N16" s="33">
+      <c r="N16" s="34">
         <v>2</v>
       </c>
-      <c r="O16" s="33">
+      <c r="O16" s="34">
         <v>3</v>
       </c>
-      <c r="P16" s="33">
+      <c r="P16" s="34">
         <v>4</v>
       </c>
-      <c r="Q16" s="33">
+      <c r="Q16" s="34">
         <v>5</v>
       </c>
-      <c r="R16" s="33">
+      <c r="R16" s="34">
         <v>6</v>
       </c>
-      <c r="S16" s="34">
+      <c r="S16" s="35">
         <v>7</v>
       </c>
     </row>
     <row r="18" spans="2:34" ht="17" thickBot="1"/>
     <row r="19" spans="2:34" ht="17" thickBot="1">
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="D19" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="E19" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="22" t="s">
+      <c r="F19" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="G19" s="18" t="s">
+      <c r="G19" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="19" t="s">
+      <c r="H19" s="20" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="20" spans="2:34" ht="18">
-      <c r="C20" s="17"/>
-      <c r="F20" s="17"/>
+      <c r="C20" s="18"/>
+      <c r="F20" s="18"/>
     </row>
     <row r="21" spans="2:34">
       <c r="AH21" t="s">
@@ -13112,31 +15049,31 @@
     </row>
     <row r="24" spans="2:34" ht="17" thickBot="1"/>
     <row r="25" spans="2:34" ht="17" thickBot="1">
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C25" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="19" t="s">
+      <c r="D25" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="E25" s="20" t="s">
+      <c r="E25" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="F25" s="15" t="s">
+      <c r="F25" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G25" s="15" t="s">
+      <c r="G25" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="H25" s="16" t="s">
+      <c r="H25" s="17" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="26" spans="2:34" ht="18">
-      <c r="C26" s="17"/>
-      <c r="F26" s="17"/>
+      <c r="C26" s="18"/>
+      <c r="F26" s="18"/>
     </row>
     <row r="29" spans="2:34" ht="17" thickBot="1">
       <c r="AH29" t="s">
@@ -13144,792 +15081,1768 @@
       </c>
     </row>
     <row r="30" spans="2:34" ht="17" thickBot="1">
-      <c r="B30" s="21" t="s">
+      <c r="B30" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="22" t="s">
+      <c r="C30" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="D30" s="23" t="s">
+      <c r="D30" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="E30" s="21" t="s">
+      <c r="E30" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F30" s="15" t="s">
+      <c r="F30" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="G30" s="15" t="s">
+      <c r="G30" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="H30" s="16" t="s">
+      <c r="H30" s="17" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="31" spans="2:34" ht="18">
-      <c r="C31" s="17"/>
-      <c r="F31" s="17"/>
+      <c r="C31" s="18"/>
+      <c r="F31" s="18"/>
     </row>
     <row r="35" spans="2:10" ht="17" thickBot="1"/>
     <row r="36" spans="2:10" ht="17" thickBot="1">
-      <c r="C36" s="47" t="s">
+      <c r="C36" s="48" t="s">
         <v>29</v>
       </c>
-      <c r="E36" s="38"/>
-      <c r="H36" s="47" t="s">
+      <c r="E36" s="39"/>
+      <c r="H36" s="48" t="s">
         <v>46</v>
       </c>
-      <c r="J36" s="38"/>
+      <c r="J36" s="39"/>
     </row>
     <row r="37" spans="2:10" ht="19" customHeight="1" thickBot="1">
-      <c r="B37" s="42" t="s">
+      <c r="B37" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="C37" s="45" t="s">
+      <c r="C37" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="D37" s="44" t="s">
+      <c r="D37" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="E37" s="43"/>
-      <c r="G37" s="42"/>
-      <c r="H37" s="42" t="s">
+      <c r="E37" s="44"/>
+      <c r="G37" s="43"/>
+      <c r="H37" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="I37" s="45" t="s">
+      <c r="I37" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="J37" s="44" t="s">
+      <c r="J37" s="45" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="38" spans="2:10">
-      <c r="B38" s="40" t="s">
+      <c r="B38" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="C38" s="1" t="s">
+      <c r="C38" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D38" s="39" t="s">
+      <c r="D38" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="E38" s="40" t="s">
+      <c r="E38" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="G38" s="40" t="s">
+      <c r="G38" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="H38" s="40" t="s">
+      <c r="H38" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="I38" s="46" t="s">
+      <c r="I38" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="J38" s="41" t="s">
+      <c r="J38" s="42" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="39" spans="2:10">
-      <c r="B39" s="1" t="s">
+      <c r="B39" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="C39" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D39" s="39" t="s">
+      <c r="D39" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="E39" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G39" s="1" t="s">
+      <c r="G39" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H39" s="1" t="s">
+      <c r="H39" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I39" s="25" t="s">
+      <c r="I39" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="J39" s="39" t="s">
+      <c r="J39" s="40" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="40" spans="2:10">
-      <c r="B40" s="1" t="s">
+      <c r="B40" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C40" s="40" t="s">
+      <c r="C40" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="D40" s="41" t="s">
+      <c r="D40" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="E40" s="1"/>
-      <c r="G40" s="1" t="s">
+      <c r="E40" s="2"/>
+      <c r="G40" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="H40" s="1" t="s">
+      <c r="H40" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I40" s="25" t="s">
+      <c r="I40" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="J40" s="1" t="s">
+      <c r="J40" s="2" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="41" spans="2:10">
-      <c r="B41" s="1" t="s">
+      <c r="B41" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C41" s="1" t="s">
+      <c r="C41" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D41" s="39" t="s">
+      <c r="D41" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="E41" s="1"/>
-      <c r="G41" s="1"/>
-      <c r="H41" s="1" t="s">
+      <c r="E41" s="2"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I41" s="25" t="s">
+      <c r="I41" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="J41" s="1" t="s">
+      <c r="J41" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="42" spans="2:10">
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C42" s="1" t="s">
+      <c r="C42" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D42" s="39" t="s">
+      <c r="D42" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E42" s="1"/>
-      <c r="G42" s="1"/>
-      <c r="H42" s="1" t="s">
+      <c r="E42" s="2"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I42" s="39" t="s">
+      <c r="I42" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="J42" s="1"/>
+      <c r="J42" s="2"/>
     </row>
     <row r="43" spans="2:10">
-      <c r="B43" s="1"/>
-      <c r="C43" s="1" t="s">
+      <c r="B43" s="2"/>
+      <c r="C43" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D43" s="39" t="s">
+      <c r="D43" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="E43" s="1"/>
-      <c r="G43" s="1"/>
-      <c r="H43" s="25" t="s">
+      <c r="E43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="26" t="s">
         <v>0</v>
       </c>
-      <c r="I43" s="39" t="s">
+      <c r="I43" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="J43" s="1"/>
+      <c r="J43" s="2"/>
     </row>
     <row r="44" spans="2:10">
-      <c r="B44" s="1"/>
-      <c r="C44" s="1" t="s">
+      <c r="B44" s="2"/>
+      <c r="C44" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D44" s="39" t="s">
+      <c r="D44" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="E44" s="1"/>
-      <c r="G44" s="1"/>
-      <c r="H44" s="25" t="s">
+      <c r="E44" s="2"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="I44" s="39" t="s">
+      <c r="I44" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="J44" s="1"/>
+      <c r="J44" s="2"/>
     </row>
     <row r="45" spans="2:10" ht="17" thickBot="1"/>
     <row r="46" spans="2:10" ht="17" thickBot="1">
-      <c r="C46" s="47" t="s">
+      <c r="C46" s="48" t="s">
         <v>48</v>
       </c>
-      <c r="E46" s="38"/>
-      <c r="H46" s="47" t="s">
+      <c r="E46" s="39"/>
+      <c r="H46" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="J46" s="38"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="2:10" ht="20" customHeight="1" thickBot="1">
-      <c r="B47" s="42" t="s">
+      <c r="B47" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="C47" s="45" t="s">
+      <c r="C47" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="D47" s="44" t="s">
+      <c r="D47" s="45" t="s">
         <v>30</v>
       </c>
-      <c r="E47" s="43"/>
-      <c r="G47" s="42"/>
-      <c r="H47" s="42" t="s">
+      <c r="E47" s="44"/>
+      <c r="G47" s="43"/>
+      <c r="H47" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="I47" s="45" t="s">
+      <c r="I47" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="J47" s="44" t="s">
+      <c r="J47" s="45" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="48" spans="2:10">
-      <c r="B48" s="40" t="s">
+      <c r="B48" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="C48" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D48" s="39" t="s">
+      <c r="D48" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="E48" s="40" t="s">
+      <c r="E48" s="41" t="s">
         <v>43</v>
       </c>
-      <c r="G48" s="40" t="s">
+      <c r="G48" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="H48" s="1" t="s">
+      <c r="H48" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="I48" s="41" t="s">
+      <c r="I48" s="42" t="s">
         <v>1</v>
       </c>
-      <c r="J48" s="39" t="s">
+      <c r="J48" s="40" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="49" spans="2:21">
-      <c r="B49" s="1" t="s">
+      <c r="B49" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="C49" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D49" s="39" t="s">
+      <c r="D49" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="E49" s="40" t="s">
+      <c r="E49" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="G49" s="1" t="s">
+      <c r="G49" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="H49" s="1" t="s">
+      <c r="H49" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="I49" s="39" t="s">
+      <c r="I49" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="J49" s="39" t="s">
+      <c r="J49" s="40" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="50" spans="2:21">
-      <c r="B50" s="1" t="s">
+      <c r="B50" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C50" s="1" t="s">
+      <c r="C50" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="D50" s="1" t="s">
+      <c r="D50" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="E50" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G50" s="1"/>
-      <c r="H50" s="1" t="s">
+      <c r="G50" s="2"/>
+      <c r="H50" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I50" s="1" t="s">
+      <c r="I50" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="J50" s="39" t="s">
+      <c r="J50" s="40" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="51" spans="2:21">
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="C51" s="1" t="s">
+      <c r="C51" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D51" s="39" t="s">
+      <c r="D51" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="E51" s="1"/>
-      <c r="G51" s="1"/>
-      <c r="H51" s="1" t="s">
+      <c r="E51" s="2"/>
+      <c r="G51" s="2"/>
+      <c r="H51" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I51" s="1" t="s">
+      <c r="I51" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J51" s="40" t="s">
+      <c r="J51" s="41" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="52" spans="2:21">
-      <c r="B52" s="1"/>
-      <c r="C52" s="1" t="s">
+      <c r="B52" s="2"/>
+      <c r="C52" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D52" s="39" t="s">
+      <c r="D52" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="E52" s="1"/>
-      <c r="G52" s="1"/>
-      <c r="H52" s="1" t="s">
+      <c r="E52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I52" s="1" t="s">
+      <c r="I52" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="J52" s="1" t="s">
+      <c r="J52" s="2" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="53" spans="2:21">
-      <c r="B53" s="1"/>
-      <c r="C53" s="1" t="s">
+      <c r="B53" s="2"/>
+      <c r="C53" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D53" s="39" t="s">
+      <c r="D53" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="E53" s="1"/>
-      <c r="G53" s="1"/>
-      <c r="H53" s="1" t="s">
+      <c r="E53" s="2"/>
+      <c r="G53" s="2"/>
+      <c r="H53" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I53" s="41" t="s">
+      <c r="I53" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="J53" s="1"/>
+      <c r="J53" s="2"/>
     </row>
     <row r="54" spans="2:21">
-      <c r="B54" s="1"/>
-      <c r="C54" s="1" t="s">
+      <c r="B54" s="2"/>
+      <c r="C54" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D54" s="39" t="s">
+      <c r="D54" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="E54" s="1"/>
-      <c r="G54" s="1"/>
-      <c r="H54" s="1" t="s">
+      <c r="E54" s="2"/>
+      <c r="G54" s="2"/>
+      <c r="H54" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="I54" s="39" t="s">
+      <c r="I54" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="J54" s="1"/>
-      <c r="R54" s="49"/>
-      <c r="S54" s="49"/>
+      <c r="J54" s="2"/>
+      <c r="R54" s="50"/>
+      <c r="S54" s="50"/>
     </row>
     <row r="55" spans="2:21">
-      <c r="C55" s="48"/>
-      <c r="R55" s="49"/>
+      <c r="C55" s="49"/>
+      <c r="R55" s="50"/>
     </row>
     <row r="59" spans="2:21" ht="17" thickBot="1"/>
     <row r="60" spans="2:21" ht="17" thickBot="1">
       <c r="N60" t="s">
-        <v>65</v>
-      </c>
-      <c r="O60" s="48"/>
-      <c r="P60" s="76" t="s">
+        <v>68</v>
+      </c>
+      <c r="O60" s="49"/>
+      <c r="P60" s="78" t="s">
         <v>53</v>
       </c>
-      <c r="Q60" s="77" t="s">
+      <c r="Q60" s="79" t="s">
         <v>54</v>
       </c>
-      <c r="R60" s="78" t="s">
+      <c r="R60" s="80" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="61" spans="2:21" ht="34">
-      <c r="O61" s="74" t="s">
+      <c r="O61" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="P61" s="79" t="s">
+      <c r="P61" s="81" t="s">
         <v>56</v>
       </c>
-      <c r="Q61" s="80" t="s">
+      <c r="Q61" s="82" t="s">
         <v>57</v>
       </c>
-      <c r="R61" s="81"/>
+      <c r="R61" s="83"/>
     </row>
     <row r="62" spans="2:21" ht="34">
-      <c r="O62" s="24" t="s">
+      <c r="O62" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="P62" s="82" t="s">
+      <c r="P62" s="84" t="s">
         <v>58</v>
       </c>
-      <c r="Q62" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="R62" s="83"/>
+      <c r="Q62" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="R62" s="85"/>
     </row>
     <row r="63" spans="2:21" ht="34">
-      <c r="O63" s="24" t="s">
+      <c r="O63" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="P63" s="82" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q63" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="R63" s="83"/>
+      <c r="P63" s="84" t="s">
+        <v>64</v>
+      </c>
+      <c r="Q63" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="R63" s="85"/>
     </row>
     <row r="64" spans="2:21" ht="34">
-      <c r="O64" s="24" t="s">
+      <c r="O64" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="P64" s="82" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q64" s="2">
+      <c r="P64" s="84" t="s">
+        <v>65</v>
+      </c>
+      <c r="Q64" s="3">
         <v>12</v>
       </c>
-      <c r="R64" s="83">
+      <c r="R64" s="85">
         <v>1</v>
       </c>
-      <c r="U64" s="48"/>
+      <c r="U64" s="49"/>
     </row>
     <row r="65" spans="15:29" ht="34">
-      <c r="O65" s="24" t="s">
+      <c r="O65" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="P65" s="82" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q65" s="2">
+      <c r="P65" s="84" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q65" s="3">
         <v>12</v>
       </c>
-      <c r="R65" s="83">
+      <c r="R65" s="85">
         <v>1</v>
       </c>
-      <c r="U65" s="48"/>
+      <c r="U65" s="49"/>
     </row>
     <row r="66" spans="15:29" ht="34">
-      <c r="O66" s="24" t="s">
+      <c r="O66" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="P66" s="82" t="s">
-        <v>64</v>
-      </c>
-      <c r="Q66" s="2"/>
-      <c r="R66" s="83" t="s">
-        <v>60</v>
+      <c r="P66" s="84" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q66" s="3"/>
+      <c r="R66" s="85" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="67" spans="15:29" ht="35" thickBot="1">
-      <c r="O67" s="75" t="s">
+      <c r="O67" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="P67" s="84" t="s">
+      <c r="P67" s="86" t="s">
         <v>57</v>
       </c>
-      <c r="Q67" s="85"/>
-      <c r="R67" s="86" t="s">
-        <v>60</v>
+      <c r="Q67" s="87"/>
+      <c r="R67" s="88" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="68" spans="15:29" ht="17" thickBot="1"/>
     <row r="69" spans="15:29" ht="17" thickBot="1">
-      <c r="T69" s="48"/>
-      <c r="U69" s="64" t="s">
+      <c r="T69" s="49"/>
+      <c r="U69" s="65" t="s">
         <v>53</v>
       </c>
-      <c r="X69" s="48"/>
-      <c r="Y69" s="64" t="s">
+      <c r="X69" s="49"/>
+      <c r="Y69" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="AB69" s="48"/>
-      <c r="AC69" s="64" t="s">
-        <v>54</v>
+      <c r="AB69" s="49"/>
+      <c r="AC69" s="65" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="70" spans="15:29" ht="17" thickBot="1">
-      <c r="T70" s="63"/>
-      <c r="V70" s="63"/>
-      <c r="X70" s="63"/>
-      <c r="Z70" s="63"/>
-      <c r="AB70" s="63"/>
+      <c r="T70" s="64"/>
+      <c r="V70" s="64"/>
+      <c r="X70" s="64"/>
+      <c r="Z70" s="64"/>
+      <c r="AB70" s="64"/>
     </row>
     <row r="71" spans="15:29" ht="17" customHeight="1" thickBot="1">
-      <c r="T71" s="64" t="s">
-        <v>78</v>
-      </c>
-      <c r="U71" s="65"/>
-      <c r="V71" s="63"/>
-      <c r="X71" s="64" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y71" s="65"/>
-      <c r="Z71" s="63"/>
-      <c r="AB71" s="64" t="s">
-        <v>78</v>
-      </c>
-      <c r="AC71" s="65"/>
+      <c r="T71" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="U71" s="66"/>
+      <c r="V71" s="64"/>
+      <c r="X71" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y71" s="66"/>
+      <c r="Z71" s="64"/>
+      <c r="AB71" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="AC71" s="66"/>
     </row>
     <row r="72" spans="15:29" ht="32" customHeight="1">
-      <c r="S72" s="87" t="s">
-        <v>74</v>
-      </c>
-      <c r="T72" s="66">
+      <c r="S72" s="89" t="s">
+        <v>77</v>
+      </c>
+      <c r="T72" s="67">
         <v>2</v>
       </c>
-      <c r="U72" s="54" t="s">
-        <v>66</v>
-      </c>
-      <c r="V72" s="63"/>
-      <c r="W72" s="87" t="s">
-        <v>79</v>
-      </c>
-      <c r="X72" s="66">
+      <c r="U72" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="V72" s="64"/>
+      <c r="W72" s="89" t="s">
+        <v>81</v>
+      </c>
+      <c r="X72" s="67">
         <v>8</v>
       </c>
-      <c r="Y72" s="54" t="s">
+      <c r="Y72" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="Z72" s="63"/>
-      <c r="AA72" s="87" t="s">
-        <v>80</v>
-      </c>
-      <c r="AB72" s="66">
+      <c r="Z72" s="64"/>
+      <c r="AA72" s="89" t="s">
+        <v>82</v>
+      </c>
+      <c r="AB72" s="67">
         <v>1</v>
       </c>
-      <c r="AC72" s="57" t="s">
-        <v>70</v>
+      <c r="AC72" s="58" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="73" spans="15:29" ht="18" thickBot="1">
-      <c r="S73" s="88"/>
-      <c r="T73" s="67">
+      <c r="S73" s="90"/>
+      <c r="T73" s="68">
         <v>4</v>
       </c>
-      <c r="U73" s="55" t="s">
-        <v>67</v>
-      </c>
-      <c r="V73" s="63"/>
-      <c r="W73" s="88"/>
-      <c r="X73" s="67">
+      <c r="U73" s="56" t="s">
+        <v>70</v>
+      </c>
+      <c r="V73" s="64"/>
+      <c r="W73" s="90"/>
+      <c r="X73" s="68">
         <v>10</v>
       </c>
-      <c r="Y73" s="55" t="s">
-        <v>72</v>
-      </c>
-      <c r="Z73" s="63"/>
-      <c r="AB73" s="68">
+      <c r="Y73" s="56" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z73" s="64"/>
+      <c r="AB73" s="69">
         <v>3</v>
       </c>
-      <c r="AC73" s="59" t="s">
-        <v>71</v>
+      <c r="AC73" s="60" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="74" spans="15:29" ht="18" thickBot="1">
-      <c r="S74" s="88"/>
-      <c r="T74" s="68">
+      <c r="S74" s="90"/>
+      <c r="T74" s="69">
         <v>6</v>
       </c>
-      <c r="U74" s="56" t="s">
-        <v>68</v>
-      </c>
-      <c r="V74" s="63"/>
-      <c r="W74" s="88"/>
-      <c r="X74" s="68">
+      <c r="U74" s="57" t="s">
+        <v>71</v>
+      </c>
+      <c r="V74" s="64"/>
+      <c r="W74" s="90"/>
+      <c r="X74" s="69">
         <v>12</v>
       </c>
-      <c r="Y74" s="56" t="s">
-        <v>73</v>
-      </c>
-      <c r="Z74" s="63"/>
-      <c r="AA74" s="65"/>
-      <c r="AB74" s="50"/>
+      <c r="Y74" s="57" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z74" s="64"/>
+      <c r="AA74" s="66"/>
+      <c r="AB74" s="51"/>
     </row>
     <row r="75" spans="15:29" ht="4" customHeight="1" thickBot="1">
-      <c r="S75" s="88"/>
-      <c r="T75" s="63"/>
-      <c r="U75" s="63"/>
-      <c r="V75" s="63"/>
-      <c r="W75" s="88"/>
-      <c r="X75" s="63"/>
-      <c r="Y75" s="63"/>
-      <c r="Z75" s="63"/>
-      <c r="AA75" s="53"/>
-      <c r="AB75" s="63"/>
+      <c r="S75" s="90"/>
+      <c r="T75" s="64"/>
+      <c r="U75" s="64"/>
+      <c r="V75" s="64"/>
+      <c r="W75" s="90"/>
+      <c r="X75" s="64"/>
+      <c r="Y75" s="64"/>
+      <c r="Z75" s="64"/>
+      <c r="AA75" s="54"/>
+      <c r="AB75" s="64"/>
     </row>
     <row r="76" spans="15:29" ht="36" customHeight="1" thickBot="1">
-      <c r="S76" s="87" t="s">
-        <v>77</v>
-      </c>
-      <c r="T76" s="66">
+      <c r="S76" s="89" t="s">
+        <v>79</v>
+      </c>
+      <c r="T76" s="67">
         <v>8</v>
       </c>
-      <c r="U76" s="57" t="s">
-        <v>69</v>
-      </c>
-      <c r="V76" s="63"/>
-      <c r="W76" s="87" t="s">
-        <v>74</v>
-      </c>
-      <c r="X76" s="69">
+      <c r="U76" s="58" t="s">
+        <v>72</v>
+      </c>
+      <c r="V76" s="64"/>
+      <c r="W76" s="89" t="s">
+        <v>101</v>
+      </c>
+      <c r="X76" s="70">
         <v>13</v>
       </c>
-      <c r="Y76" s="62" t="s">
+      <c r="Y76" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="Z76" s="63"/>
-      <c r="AA76" s="53"/>
-      <c r="AB76" s="63"/>
+      <c r="Z76" s="64"/>
+      <c r="AA76" s="54"/>
+      <c r="AB76" s="64"/>
     </row>
     <row r="77" spans="15:29" ht="17">
-      <c r="S77" s="88"/>
-      <c r="T77" s="67">
+      <c r="S77" s="90"/>
+      <c r="T77" s="68">
         <v>10</v>
       </c>
-      <c r="U77" s="58" t="s">
-        <v>70</v>
-      </c>
-      <c r="V77" s="63"/>
-      <c r="W77" s="65"/>
-      <c r="X77" s="51"/>
-      <c r="Y77" s="63"/>
-      <c r="Z77" s="63"/>
-      <c r="AA77" s="63"/>
+      <c r="U77" s="59" t="s">
+        <v>73</v>
+      </c>
+      <c r="V77" s="64"/>
+      <c r="W77" s="66"/>
+      <c r="X77" s="52"/>
+      <c r="Y77" s="64"/>
+      <c r="Z77" s="64"/>
+      <c r="AA77" s="64"/>
     </row>
     <row r="78" spans="15:29" ht="18" thickBot="1">
-      <c r="S78" s="88"/>
-      <c r="T78" s="68">
+      <c r="S78" s="90"/>
+      <c r="T78" s="69">
         <v>12</v>
       </c>
-      <c r="U78" s="59" t="s">
-        <v>71</v>
-      </c>
-      <c r="V78" s="63"/>
-      <c r="W78" s="65"/>
-      <c r="X78" s="51"/>
-      <c r="Y78" s="63"/>
-      <c r="Z78" s="63"/>
-      <c r="AA78" s="63"/>
+      <c r="U78" s="60" t="s">
+        <v>74</v>
+      </c>
+      <c r="V78" s="64"/>
+      <c r="W78" s="66"/>
+      <c r="X78" s="52"/>
+      <c r="Y78" s="64"/>
+      <c r="Z78" s="64"/>
+      <c r="AA78" s="64"/>
     </row>
     <row r="79" spans="15:29" ht="4" customHeight="1" thickBot="1">
-      <c r="S79" s="88"/>
-      <c r="T79" s="63"/>
-      <c r="U79" s="63"/>
-      <c r="V79" s="63"/>
-      <c r="W79" s="65"/>
-      <c r="X79" s="65"/>
-      <c r="Y79" s="63"/>
-      <c r="Z79" s="63"/>
-      <c r="AA79" s="63"/>
+      <c r="S79" s="90"/>
+      <c r="T79" s="64"/>
+      <c r="U79" s="64"/>
+      <c r="V79" s="64"/>
+      <c r="W79" s="66"/>
+      <c r="X79" s="66"/>
+      <c r="Y79" s="64"/>
+      <c r="Z79" s="64"/>
+      <c r="AA79" s="64"/>
     </row>
-    <row r="80" spans="15:29" ht="51">
-      <c r="S80" s="87" t="s">
+    <row r="80" spans="15:29" ht="36" customHeight="1">
+      <c r="S80" s="89" t="s">
+        <v>78</v>
+      </c>
+      <c r="T80" s="67">
+        <v>7</v>
+      </c>
+      <c r="U80" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="V80" s="64"/>
+      <c r="W80" s="66"/>
+      <c r="X80" s="51"/>
+      <c r="Y80" s="64"/>
+      <c r="Z80" s="64"/>
+      <c r="AA80" s="64"/>
+    </row>
+    <row r="81" spans="14:31" ht="17">
+      <c r="S81" s="90"/>
+      <c r="T81" s="71">
+        <v>9</v>
+      </c>
+      <c r="U81" s="61" t="s">
+        <v>70</v>
+      </c>
+      <c r="V81" s="64"/>
+      <c r="W81" s="72"/>
+      <c r="X81" s="53"/>
+      <c r="Y81" s="64"/>
+      <c r="Z81" s="64"/>
+      <c r="AA81" s="64"/>
+    </row>
+    <row r="82" spans="14:31" ht="18" thickBot="1">
+      <c r="S82" s="90"/>
+      <c r="T82" s="73">
+        <v>11</v>
+      </c>
+      <c r="U82" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="V82" s="64"/>
+      <c r="W82" s="72"/>
+      <c r="X82" s="53"/>
+      <c r="Y82" s="64"/>
+      <c r="Z82" s="64"/>
+      <c r="AA82" s="64"/>
+    </row>
+    <row r="83" spans="14:31" ht="4" customHeight="1" thickBot="1">
+      <c r="S83" s="90"/>
+      <c r="T83" s="66"/>
+      <c r="U83" s="66"/>
+      <c r="V83" s="64"/>
+      <c r="W83" s="64"/>
+      <c r="X83" s="64"/>
+      <c r="Y83" s="64"/>
+      <c r="Z83" s="64"/>
+      <c r="AA83" s="64"/>
+    </row>
+    <row r="84" spans="14:31" ht="35" thickBot="1">
+      <c r="S84" s="89" t="s">
+        <v>100</v>
+      </c>
+      <c r="T84" s="70">
+        <v>13</v>
+      </c>
+      <c r="U84" s="75" t="s">
+        <v>72</v>
+      </c>
+      <c r="V84" s="64"/>
+      <c r="W84" s="64"/>
+      <c r="X84" s="64"/>
+      <c r="Y84" s="64"/>
+      <c r="Z84" s="64"/>
+      <c r="AA84" s="64"/>
+    </row>
+    <row r="85" spans="14:31" ht="17" thickBot="1">
+      <c r="T85" s="64"/>
+      <c r="U85" s="64"/>
+      <c r="V85" s="64"/>
+      <c r="W85" s="64"/>
+      <c r="X85" s="64"/>
+      <c r="Y85" s="64"/>
+      <c r="Z85" s="64"/>
+      <c r="AA85" s="64"/>
+    </row>
+    <row r="86" spans="14:31" ht="17" thickBot="1">
+      <c r="N86" t="s">
+        <v>83</v>
+      </c>
+      <c r="O86" s="49"/>
+      <c r="P86" s="91" t="s">
+        <v>55</v>
+      </c>
+      <c r="Q86" s="92" t="s">
+        <v>84</v>
+      </c>
+      <c r="R86" s="49"/>
+    </row>
+    <row r="87" spans="14:31" ht="17">
+      <c r="O87" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="P87" s="81" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q87" s="93"/>
+      <c r="R87" s="54"/>
+    </row>
+    <row r="88" spans="14:31" ht="34">
+      <c r="O88" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="P88" s="84" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q88" s="85"/>
+      <c r="R88" s="54"/>
+    </row>
+    <row r="89" spans="14:31" ht="32" customHeight="1">
+      <c r="O89" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="P89" s="84" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q89" s="85"/>
+      <c r="R89" s="54"/>
+    </row>
+    <row r="90" spans="14:31" ht="34">
+      <c r="O90" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="P90" s="84" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q90" s="85"/>
+      <c r="R90" s="54"/>
+      <c r="U90" s="49"/>
+    </row>
+    <row r="91" spans="14:31" ht="34">
+      <c r="O91" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="P91" s="84" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q91" s="85">
+        <v>13</v>
+      </c>
+      <c r="R91" s="54"/>
+      <c r="U91" s="49"/>
+    </row>
+    <row r="92" spans="14:31" ht="34">
+      <c r="O92" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="P92" s="84" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q92" s="85" t="s">
+        <v>62</v>
+      </c>
+      <c r="R92" s="54"/>
+    </row>
+    <row r="93" spans="14:31" ht="35" thickBot="1">
+      <c r="O93" s="77" t="s">
+        <v>5</v>
+      </c>
+      <c r="P93" s="86" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q93" s="88" t="s">
+        <v>61</v>
+      </c>
+      <c r="R93" s="54"/>
+      <c r="AA93" s="49"/>
+      <c r="AB93" s="49"/>
+      <c r="AC93" s="49"/>
+      <c r="AD93" s="49"/>
+      <c r="AE93" s="49"/>
+    </row>
+    <row r="94" spans="14:31" ht="17" thickBot="1">
+      <c r="AA94" s="49"/>
+      <c r="AB94" s="49"/>
+      <c r="AC94" s="49"/>
+      <c r="AD94" s="49"/>
+      <c r="AE94" s="49"/>
+    </row>
+    <row r="95" spans="14:31" ht="17" thickBot="1">
+      <c r="T95" s="49"/>
+      <c r="U95" s="65" t="s">
+        <v>55</v>
+      </c>
+      <c r="X95" s="49"/>
+      <c r="Y95" s="65" t="s">
+        <v>84</v>
+      </c>
+      <c r="AA95" s="49"/>
+      <c r="AB95" s="49"/>
+      <c r="AC95" s="74"/>
+      <c r="AD95" s="49"/>
+      <c r="AE95" s="49"/>
+    </row>
+    <row r="96" spans="14:31" ht="17" thickBot="1">
+      <c r="T96" s="64"/>
+      <c r="V96" s="64"/>
+      <c r="X96" s="64"/>
+      <c r="Z96" s="64"/>
+      <c r="AA96" s="49"/>
+      <c r="AB96" s="66"/>
+      <c r="AC96" s="49"/>
+      <c r="AD96" s="49"/>
+      <c r="AE96" s="49"/>
+    </row>
+    <row r="97" spans="19:31" ht="17" thickBot="1">
+      <c r="T97" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="U97" s="66"/>
+      <c r="V97" s="64"/>
+      <c r="X97" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y97" s="66"/>
+      <c r="Z97" s="64"/>
+      <c r="AA97" s="49"/>
+      <c r="AB97" s="74"/>
+      <c r="AC97" s="66"/>
+      <c r="AD97" s="49"/>
+      <c r="AE97" s="49"/>
+    </row>
+    <row r="98" spans="19:31" ht="31" customHeight="1">
+      <c r="S98" s="89" t="s">
+        <v>99</v>
+      </c>
+      <c r="T98" s="67">
+        <v>2</v>
+      </c>
+      <c r="U98" s="58" t="s">
+        <v>5</v>
+      </c>
+      <c r="V98" s="64"/>
+      <c r="W98" s="89" t="s">
+        <v>102</v>
+      </c>
+      <c r="X98" s="67">
+        <v>9</v>
+      </c>
+      <c r="Y98" s="58" t="s">
+        <v>5</v>
+      </c>
+      <c r="Z98" s="64"/>
+      <c r="AA98" s="52"/>
+      <c r="AB98" s="66"/>
+      <c r="AC98" s="52"/>
+      <c r="AD98" s="49"/>
+      <c r="AE98" s="49"/>
+    </row>
+    <row r="99" spans="19:31" ht="17">
+      <c r="S99" s="90"/>
+      <c r="T99" s="68">
+        <v>4</v>
+      </c>
+      <c r="U99" s="59" t="s">
+        <v>74</v>
+      </c>
+      <c r="V99" s="64"/>
+      <c r="W99" s="90"/>
+      <c r="X99" s="68">
+        <v>11</v>
+      </c>
+      <c r="Y99" s="59" t="s">
+        <v>74</v>
+      </c>
+      <c r="Z99" s="64"/>
+      <c r="AA99" s="49"/>
+      <c r="AB99" s="66"/>
+      <c r="AC99" s="52"/>
+      <c r="AD99" s="49"/>
+      <c r="AE99" s="49"/>
+    </row>
+    <row r="100" spans="19:31" ht="18" thickBot="1">
+      <c r="S100" s="90"/>
+      <c r="T100" s="68">
+        <v>6</v>
+      </c>
+      <c r="U100" s="59" t="s">
+        <v>91</v>
+      </c>
+      <c r="V100" s="64"/>
+      <c r="W100" s="90"/>
+      <c r="X100" s="69">
+        <v>13</v>
+      </c>
+      <c r="Y100" s="60" t="s">
+        <v>91</v>
+      </c>
+      <c r="Z100" s="64"/>
+      <c r="AA100" s="66"/>
+      <c r="AB100" s="51"/>
+      <c r="AC100" s="49"/>
+      <c r="AD100" s="49"/>
+      <c r="AE100" s="49"/>
+    </row>
+    <row r="101" spans="19:31" ht="17">
+      <c r="S101" s="90"/>
+      <c r="T101" s="68">
+        <v>8</v>
+      </c>
+      <c r="U101" s="59" t="s">
+        <v>73</v>
+      </c>
+      <c r="V101" s="64"/>
+      <c r="W101" s="90"/>
+      <c r="X101" s="64"/>
+      <c r="Y101" s="64"/>
+      <c r="Z101" s="64"/>
+      <c r="AA101" s="54"/>
+      <c r="AB101" s="66"/>
+      <c r="AC101" s="49"/>
+      <c r="AD101" s="49"/>
+      <c r="AE101" s="49"/>
+    </row>
+    <row r="102" spans="19:31" ht="17" customHeight="1">
+      <c r="S102" s="89"/>
+      <c r="T102" s="68">
+        <v>10</v>
+      </c>
+      <c r="U102" s="59" t="s">
+        <v>92</v>
+      </c>
+      <c r="V102" s="64"/>
+      <c r="W102" s="52"/>
+      <c r="X102" s="72"/>
+      <c r="Y102" s="53"/>
+      <c r="Z102" s="64"/>
+      <c r="AA102" s="54"/>
+      <c r="AB102" s="66"/>
+      <c r="AC102" s="49"/>
+      <c r="AD102" s="49"/>
+      <c r="AE102" s="49"/>
+    </row>
+    <row r="103" spans="19:31" ht="18" thickBot="1">
+      <c r="S103" s="90"/>
+      <c r="T103" s="69">
+        <v>12</v>
+      </c>
+      <c r="U103" s="60" t="s">
+        <v>72</v>
+      </c>
+      <c r="V103" s="64"/>
+      <c r="W103" s="66"/>
+      <c r="X103" s="52"/>
+      <c r="Y103" s="64"/>
+      <c r="Z103" s="64"/>
+      <c r="AA103" s="64"/>
+    </row>
+    <row r="104" spans="19:31" ht="3" customHeight="1" thickBot="1">
+      <c r="S104" s="90"/>
+      <c r="V104" s="64"/>
+      <c r="W104" s="66"/>
+      <c r="X104" s="52"/>
+      <c r="Y104" s="64"/>
+      <c r="Z104" s="64"/>
+      <c r="AA104" s="64"/>
+    </row>
+    <row r="105" spans="19:31" ht="33" customHeight="1">
+      <c r="S105" s="89" t="s">
+        <v>94</v>
+      </c>
+      <c r="T105" s="67">
+        <v>1</v>
+      </c>
+      <c r="U105" s="58" t="s">
+        <v>73</v>
+      </c>
+      <c r="V105" s="64"/>
+      <c r="W105" s="66"/>
+      <c r="X105" s="66"/>
+      <c r="Y105" s="64"/>
+      <c r="Z105" s="64"/>
+      <c r="AA105" s="64"/>
+    </row>
+    <row r="106" spans="19:31" ht="40" customHeight="1">
+      <c r="S106" s="90"/>
+      <c r="T106" s="71">
+        <v>3</v>
+      </c>
+      <c r="U106" s="96" t="s">
+        <v>92</v>
+      </c>
+      <c r="V106" s="64"/>
+      <c r="W106" s="66"/>
+      <c r="X106" s="51"/>
+      <c r="Y106" s="64"/>
+      <c r="Z106" s="64"/>
+      <c r="AA106" s="64"/>
+    </row>
+    <row r="107" spans="19:31" ht="17">
+      <c r="S107" s="90"/>
+      <c r="T107" s="71">
+        <v>5</v>
+      </c>
+      <c r="U107" s="96" t="s">
+        <v>72</v>
+      </c>
+      <c r="V107" s="64"/>
+      <c r="W107" s="72"/>
+      <c r="X107" s="53"/>
+      <c r="Y107" s="64"/>
+      <c r="Z107" s="64"/>
+      <c r="AA107" s="64"/>
+    </row>
+    <row r="108" spans="19:31" ht="17" thickBot="1">
+      <c r="S108" s="90"/>
+      <c r="T108" s="73">
+        <v>7</v>
+      </c>
+      <c r="U108" s="97" t="s">
+        <v>93</v>
+      </c>
+      <c r="V108" s="64"/>
+      <c r="W108" s="72"/>
+      <c r="X108" s="53"/>
+      <c r="Y108" s="64"/>
+      <c r="Z108" s="64"/>
+      <c r="AA108" s="64"/>
+    </row>
+    <row r="109" spans="19:31" ht="3" customHeight="1" thickBot="1">
+      <c r="V109" s="64"/>
+      <c r="W109" s="64"/>
+      <c r="X109" s="64"/>
+      <c r="Y109" s="64"/>
+      <c r="Z109" s="64"/>
+      <c r="AA109" s="64"/>
+    </row>
+    <row r="110" spans="19:31" ht="34">
+      <c r="S110" s="89" t="s">
+        <v>103</v>
+      </c>
+      <c r="T110" s="94">
+        <v>9</v>
+      </c>
+      <c r="U110" s="98" t="s">
+        <v>71</v>
+      </c>
+      <c r="V110" s="64"/>
+      <c r="W110" s="64"/>
+      <c r="X110" s="64"/>
+      <c r="Y110" s="64"/>
+      <c r="Z110" s="64"/>
+      <c r="AA110" s="64"/>
+    </row>
+    <row r="111" spans="19:31" ht="40" customHeight="1">
+      <c r="T111" s="71">
+        <v>11</v>
+      </c>
+      <c r="U111" s="99" t="s">
         <v>76</v>
       </c>
-      <c r="T80" s="66">
+    </row>
+    <row r="112" spans="19:31" ht="17" thickBot="1">
+      <c r="T112" s="73">
+        <v>13</v>
+      </c>
+      <c r="U112" s="100" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="114" spans="14:25">
+      <c r="U114" s="1"/>
+    </row>
+    <row r="115" spans="14:25" ht="17" thickBot="1"/>
+    <row r="116" spans="14:25" ht="17" thickBot="1">
+      <c r="N116" t="s">
+        <v>95</v>
+      </c>
+      <c r="O116" s="49"/>
+      <c r="P116" s="91" t="s">
+        <v>53</v>
+      </c>
+      <c r="Q116" s="92" t="s">
+        <v>55</v>
+      </c>
+      <c r="R116" s="49"/>
+    </row>
+    <row r="117" spans="14:25" ht="17">
+      <c r="O117" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="P117" s="81" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q117" s="93"/>
+      <c r="R117" s="54"/>
+    </row>
+    <row r="118" spans="14:25">
+      <c r="O118" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="P118" s="84">
+        <v>1</v>
+      </c>
+      <c r="Q118" s="85">
+        <v>12</v>
+      </c>
+      <c r="R118" s="54"/>
+    </row>
+    <row r="119" spans="14:25">
+      <c r="O119" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="P119" s="84"/>
+      <c r="Q119" s="85" t="s">
+        <v>60</v>
+      </c>
+      <c r="R119" s="54"/>
+    </row>
+    <row r="120" spans="14:25" ht="34">
+      <c r="O120" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="P120" s="84"/>
+      <c r="Q120" s="101" t="s">
+        <v>57</v>
+      </c>
+      <c r="R120" s="54"/>
+      <c r="U120" s="49"/>
+    </row>
+    <row r="121" spans="14:25" ht="34">
+      <c r="O121" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="P121" s="84"/>
+      <c r="Q121" s="101" t="s">
+        <v>67</v>
+      </c>
+      <c r="R121" s="54"/>
+      <c r="U121" s="49"/>
+    </row>
+    <row r="122" spans="14:25" ht="34">
+      <c r="O122" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="P122" s="84"/>
+      <c r="Q122" s="101" t="s">
+        <v>96</v>
+      </c>
+      <c r="R122" s="54"/>
+    </row>
+    <row r="123" spans="14:25" ht="35" thickBot="1">
+      <c r="O123" s="77" t="s">
+        <v>5</v>
+      </c>
+      <c r="P123" s="86"/>
+      <c r="Q123" s="102" t="s">
+        <v>97</v>
+      </c>
+      <c r="R123" s="54"/>
+    </row>
+    <row r="124" spans="14:25" ht="17" thickBot="1"/>
+    <row r="125" spans="14:25" ht="17" thickBot="1">
+      <c r="T125" s="49"/>
+      <c r="U125" s="65" t="s">
+        <v>53</v>
+      </c>
+      <c r="X125" s="49"/>
+      <c r="Y125" s="65" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="126" spans="14:25" ht="17" thickBot="1">
+      <c r="T126" s="64"/>
+      <c r="V126" s="64"/>
+      <c r="X126" s="64"/>
+    </row>
+    <row r="127" spans="14:25" ht="17" thickBot="1">
+      <c r="T127" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="U127" s="66"/>
+      <c r="V127" s="64"/>
+      <c r="X127" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y127" s="66"/>
+    </row>
+    <row r="128" spans="14:25" ht="37" customHeight="1">
+      <c r="S128" s="89" t="s">
+        <v>98</v>
+      </c>
+      <c r="T128" s="67">
+        <v>1</v>
+      </c>
+      <c r="U128" s="55" t="s">
+        <v>69</v>
+      </c>
+      <c r="V128" s="64"/>
+      <c r="W128" s="89" t="s">
+        <v>102</v>
+      </c>
+      <c r="X128" s="67">
+        <v>2</v>
+      </c>
+      <c r="Y128" s="58" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="129" spans="14:25" ht="18" thickBot="1">
+      <c r="S129" s="90"/>
+      <c r="T129" s="69">
+        <v>3</v>
+      </c>
+      <c r="U129" s="57" t="s">
+        <v>0</v>
+      </c>
+      <c r="V129" s="64"/>
+      <c r="W129" s="90"/>
+      <c r="X129" s="68">
+        <v>4</v>
+      </c>
+      <c r="Y129" s="59" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="130" spans="14:25" ht="17">
+      <c r="S130" s="90"/>
+      <c r="T130" s="66"/>
+      <c r="U130" s="52"/>
+      <c r="V130" s="64"/>
+      <c r="W130" s="90"/>
+      <c r="X130" s="68">
+        <v>6</v>
+      </c>
+      <c r="Y130" s="59" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="131" spans="14:25" ht="17">
+      <c r="S131" s="90"/>
+      <c r="T131" s="66"/>
+      <c r="U131" s="52"/>
+      <c r="V131" s="64"/>
+      <c r="W131" s="90"/>
+      <c r="X131" s="68">
+        <v>8</v>
+      </c>
+      <c r="Y131" s="59" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="132" spans="14:25" ht="17">
+      <c r="S132" s="89"/>
+      <c r="T132" s="66"/>
+      <c r="U132" s="52"/>
+      <c r="V132" s="64"/>
+      <c r="W132" s="89"/>
+      <c r="X132" s="68">
+        <v>10</v>
+      </c>
+      <c r="Y132" s="59" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="133" spans="14:25" ht="18" thickBot="1">
+      <c r="S133" s="90"/>
+      <c r="T133" s="66"/>
+      <c r="U133" s="52"/>
+      <c r="V133" s="64"/>
+      <c r="W133" s="90"/>
+      <c r="X133" s="69">
+        <v>12</v>
+      </c>
+      <c r="Y133" s="60" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="134" spans="14:25" ht="2" customHeight="1" thickBot="1">
+      <c r="S134" s="90"/>
+      <c r="V134" s="64"/>
+      <c r="W134" s="90"/>
+    </row>
+    <row r="135" spans="14:25" ht="34">
+      <c r="S135" s="90"/>
+      <c r="T135" s="64"/>
+      <c r="U135" s="64"/>
+      <c r="V135" s="64"/>
+      <c r="W135" s="89" t="s">
+        <v>104</v>
+      </c>
+      <c r="X135" s="67">
         <v>7</v>
       </c>
-      <c r="U80" s="54" t="s">
-        <v>66</v>
-      </c>
-      <c r="V80" s="63"/>
-      <c r="W80" s="65"/>
-      <c r="X80" s="50"/>
-      <c r="Y80" s="63"/>
-      <c r="Z80" s="63"/>
-      <c r="AA80" s="63"/>
+      <c r="Y135" s="58" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="81" spans="19:27" ht="17">
-      <c r="S81" s="88"/>
-      <c r="T81" s="70">
+    <row r="136" spans="14:25" ht="40" customHeight="1">
+      <c r="S136" s="52"/>
+      <c r="T136" s="66"/>
+      <c r="U136" s="52"/>
+      <c r="V136" s="64"/>
+      <c r="W136" s="90"/>
+      <c r="X136" s="71">
         <v>9</v>
       </c>
-      <c r="U81" s="60" t="s">
-        <v>67</v>
-      </c>
-      <c r="V81" s="63"/>
-      <c r="W81" s="71"/>
-      <c r="X81" s="52"/>
-      <c r="Y81" s="63"/>
-      <c r="Z81" s="63"/>
-      <c r="AA81" s="63"/>
+      <c r="Y136" s="96" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="82" spans="19:27" ht="18" thickBot="1">
-      <c r="S82" s="88"/>
-      <c r="T82" s="72">
+    <row r="137" spans="14:25" ht="17">
+      <c r="S137" s="103"/>
+      <c r="T137" s="72"/>
+      <c r="U137" s="104"/>
+      <c r="V137" s="64"/>
+      <c r="W137" s="90"/>
+      <c r="X137" s="71">
         <v>11</v>
       </c>
-      <c r="U82" s="61" t="s">
-        <v>68</v>
-      </c>
-      <c r="V82" s="63"/>
-      <c r="W82" s="71"/>
-      <c r="X82" s="52"/>
-      <c r="Y82" s="63"/>
-      <c r="Z82" s="63"/>
-      <c r="AA82" s="63"/>
+      <c r="Y137" s="96" t="s">
+        <v>91</v>
+      </c>
     </row>
-    <row r="83" spans="19:27" ht="4" customHeight="1" thickBot="1">
-      <c r="S83" s="88"/>
-      <c r="T83" s="65"/>
-      <c r="U83" s="65"/>
-      <c r="V83" s="63"/>
-      <c r="W83" s="63"/>
-      <c r="X83" s="63"/>
-      <c r="Y83" s="63"/>
-      <c r="Z83" s="63"/>
-      <c r="AA83" s="63"/>
+    <row r="138" spans="14:25" ht="17" thickBot="1">
+      <c r="S138" s="103"/>
+      <c r="T138" s="72"/>
+      <c r="U138" s="104"/>
+      <c r="V138" s="64"/>
+      <c r="W138" s="90"/>
+      <c r="X138" s="73">
+        <v>13</v>
+      </c>
+      <c r="Y138" s="97" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="84" spans="19:27" ht="35" thickBot="1">
-      <c r="S84" s="87" t="s">
+    <row r="139" spans="14:25">
+      <c r="S139" s="103"/>
+      <c r="T139" s="72"/>
+      <c r="U139" s="103"/>
+      <c r="V139" s="64"/>
+    </row>
+    <row r="140" spans="14:25">
+      <c r="S140" s="49"/>
+      <c r="T140" s="49"/>
+      <c r="U140" s="49"/>
+      <c r="V140" s="64"/>
+    </row>
+    <row r="141" spans="14:25" ht="17" thickBot="1">
+      <c r="S141" s="52"/>
+      <c r="T141" s="72"/>
+      <c r="U141" s="53"/>
+      <c r="W141" s="52"/>
+      <c r="X141" s="72"/>
+      <c r="Y141" s="53"/>
+    </row>
+    <row r="142" spans="14:25" ht="17" thickBot="1">
+      <c r="N142" t="s">
+        <v>107</v>
+      </c>
+      <c r="O142" s="49"/>
+      <c r="P142" s="91" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q142" s="92" t="s">
+        <v>53</v>
+      </c>
+      <c r="R142" s="49"/>
+    </row>
+    <row r="143" spans="14:25" ht="34">
+      <c r="O143" s="76" t="s">
+        <v>0</v>
+      </c>
+      <c r="P143" s="81" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q143" s="93" t="s">
+        <v>90</v>
+      </c>
+      <c r="R143" s="54"/>
+    </row>
+    <row r="144" spans="14:25" ht="34">
+      <c r="O144" s="25" t="s">
+        <v>2</v>
+      </c>
+      <c r="P144" s="84" t="s">
+        <v>62</v>
+      </c>
+      <c r="Q144" s="101" t="s">
+        <v>89</v>
+      </c>
+      <c r="R144" s="54"/>
+    </row>
+    <row r="145" spans="15:25" ht="34">
+      <c r="O145" s="25" t="s">
+        <v>4</v>
+      </c>
+      <c r="P145" s="84">
+        <v>13</v>
+      </c>
+      <c r="Q145" s="101" t="s">
+        <v>88</v>
+      </c>
+      <c r="R145" s="54"/>
+    </row>
+    <row r="146" spans="15:25" ht="33" customHeight="1">
+      <c r="O146" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="P146" s="84"/>
+      <c r="Q146" s="101" t="s">
+        <v>87</v>
+      </c>
+      <c r="R146" s="54"/>
+      <c r="U146" s="49"/>
+    </row>
+    <row r="147" spans="15:25" ht="34">
+      <c r="O147" s="25" t="s">
+        <v>1</v>
+      </c>
+      <c r="P147" s="84"/>
+      <c r="Q147" s="101" t="s">
+        <v>86</v>
+      </c>
+      <c r="R147" s="54"/>
+      <c r="U147" s="49"/>
+    </row>
+    <row r="148" spans="15:25" ht="34">
+      <c r="O148" s="25" t="s">
+        <v>3</v>
+      </c>
+      <c r="P148" s="84"/>
+      <c r="Q148" s="101" t="s">
+        <v>85</v>
+      </c>
+      <c r="R148" s="54"/>
+    </row>
+    <row r="149" spans="15:25" ht="18" thickBot="1">
+      <c r="O149" s="77" t="s">
+        <v>5</v>
+      </c>
+      <c r="P149" s="86"/>
+      <c r="Q149" s="102" t="s">
+        <v>59</v>
+      </c>
+      <c r="R149" s="54"/>
+    </row>
+    <row r="150" spans="15:25" ht="17" thickBot="1"/>
+    <row r="151" spans="15:25" ht="17" thickBot="1">
+      <c r="T151" s="49"/>
+      <c r="U151" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="X151" s="49"/>
+      <c r="Y151" s="65" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="152" spans="15:25" ht="17" thickBot="1">
+      <c r="T152" s="64"/>
+      <c r="V152" s="64"/>
+      <c r="X152" s="64"/>
+    </row>
+    <row r="153" spans="15:25" ht="17" thickBot="1">
+      <c r="T153" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="U153" s="66"/>
+      <c r="V153" s="64"/>
+      <c r="X153" s="65" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y153" s="66"/>
+    </row>
+    <row r="154" spans="15:25" ht="35" customHeight="1">
+      <c r="S154" s="89" t="s">
+        <v>105</v>
+      </c>
+      <c r="T154" s="67">
+        <v>9</v>
+      </c>
+      <c r="U154" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="V154" s="64"/>
+      <c r="W154" s="89" t="s">
+        <v>106</v>
+      </c>
+      <c r="X154" s="67">
+        <v>2</v>
+      </c>
+      <c r="Y154" s="55" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="155" spans="15:25" ht="17">
+      <c r="S155" s="90"/>
+      <c r="T155" s="68">
+        <v>11</v>
+      </c>
+      <c r="U155" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="V155" s="64"/>
+      <c r="W155" s="90"/>
+      <c r="X155" s="68">
+        <v>4</v>
+      </c>
+      <c r="Y155" s="56" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="156" spans="15:25" ht="18" thickBot="1">
+      <c r="S156" s="90"/>
+      <c r="T156" s="69">
+        <v>13</v>
+      </c>
+      <c r="U156" s="57" t="s">
         <v>75</v>
       </c>
-      <c r="T84" s="69">
+      <c r="V156" s="64"/>
+      <c r="W156" s="90"/>
+      <c r="X156" s="68">
+        <v>6</v>
+      </c>
+      <c r="Y156" s="56" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="157" spans="15:25" ht="17">
+      <c r="S157" s="90"/>
+      <c r="T157" s="66"/>
+      <c r="U157" s="52"/>
+      <c r="V157" s="64"/>
+      <c r="W157" s="90"/>
+      <c r="X157" s="68">
+        <v>8</v>
+      </c>
+      <c r="Y157" s="56" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="158" spans="15:25" ht="17">
+      <c r="S158" s="89"/>
+      <c r="T158" s="66"/>
+      <c r="U158" s="52"/>
+      <c r="V158" s="64"/>
+      <c r="W158" s="89"/>
+      <c r="X158" s="68">
+        <v>10</v>
+      </c>
+      <c r="Y158" s="56" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="159" spans="15:25" ht="18" thickBot="1">
+      <c r="S159" s="90"/>
+      <c r="T159" s="66"/>
+      <c r="U159" s="52"/>
+      <c r="V159" s="64"/>
+      <c r="W159" s="90"/>
+      <c r="X159" s="69">
+        <v>12</v>
+      </c>
+      <c r="Y159" s="57" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="160" spans="15:25" ht="2" customHeight="1" thickBot="1">
+      <c r="S160" s="90"/>
+      <c r="V160" s="64"/>
+      <c r="W160" s="90"/>
+    </row>
+    <row r="161" spans="19:25" ht="34">
+      <c r="S161" s="90"/>
+      <c r="T161" s="64"/>
+      <c r="U161" s="64"/>
+      <c r="V161" s="64"/>
+      <c r="W161" s="89" t="s">
+        <v>105</v>
+      </c>
+      <c r="X161" s="67">
+        <v>1</v>
+      </c>
+      <c r="Y161" s="98" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="162" spans="19:25" ht="17">
+      <c r="S162" s="52"/>
+      <c r="T162" s="66"/>
+      <c r="U162" s="52"/>
+      <c r="V162" s="64"/>
+      <c r="X162" s="71">
+        <v>3</v>
+      </c>
+      <c r="Y162" s="61" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="163" spans="19:25" ht="17">
+      <c r="S163" s="103"/>
+      <c r="T163" s="72"/>
+      <c r="U163" s="104"/>
+      <c r="V163" s="64"/>
+      <c r="X163" s="105">
+        <v>5</v>
+      </c>
+      <c r="Y163" s="106" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="164" spans="19:25" ht="19" customHeight="1" thickBot="1">
+      <c r="S164" s="103"/>
+      <c r="T164" s="72"/>
+      <c r="U164" s="104"/>
+      <c r="V164" s="64"/>
+      <c r="X164" s="69">
+        <v>7</v>
+      </c>
+      <c r="Y164" s="60" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="165" spans="19:25" ht="2" customHeight="1" thickBot="1">
+      <c r="S165" s="103"/>
+      <c r="T165" s="72"/>
+      <c r="U165" s="103"/>
+      <c r="V165" s="64"/>
+    </row>
+    <row r="166" spans="19:25" ht="34">
+      <c r="W166" s="89" t="s">
+        <v>108</v>
+      </c>
+      <c r="X166" s="94">
+        <v>9</v>
+      </c>
+      <c r="Y166" s="95" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="167" spans="19:25" ht="17">
+      <c r="W167" s="90"/>
+      <c r="X167" s="71">
+        <v>11</v>
+      </c>
+      <c r="Y167" s="96" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="168" spans="19:25" ht="17" thickBot="1">
+      <c r="X168" s="73">
         <v>13</v>
       </c>
-      <c r="U84" s="73" t="s">
-        <v>69</v>
-      </c>
-      <c r="V84" s="63"/>
-      <c r="W84" s="63"/>
-      <c r="X84" s="63"/>
-      <c r="Y84" s="63"/>
-      <c r="Z84" s="63"/>
-      <c r="AA84" s="63"/>
+      <c r="Y168" s="97" t="s">
+        <v>73</v>
+      </c>
     </row>
-    <row r="85" spans="19:27">
-      <c r="T85" s="63"/>
-      <c r="U85" s="63"/>
-      <c r="V85" s="63"/>
-      <c r="W85" s="63"/>
-      <c r="X85" s="63"/>
-      <c r="Y85" s="63"/>
-      <c r="Z85" s="63"/>
-      <c r="AA85" s="63"/>
+    <row r="169" spans="19:25">
+      <c r="W169" s="90"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>